<commit_message>
Revised water eqs and inputs per DrJP
</commit_message>
<xml_diff>
--- a/eastMaui/rawData/EMauiAllData.xlsx
+++ b/eastMaui/rawData/EMauiAllData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danwa\Documents\Programming\Trutta\HSHEP\EMaui\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danwa\Documents\Programming\Trutta\HSHEP\EMaui\EMpackage\eastMaui\rawData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8915D38-FE5E-4DD9-8700-40CD4CBA4028}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A65D13D4-E2C2-4BB8-A152-6A2D090C6181}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="901" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF01000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="901" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF01000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CatchSummary_deltaP" sheetId="10" r:id="rId1"/>
@@ -25,12 +25,12 @@
   <definedNames>
     <definedName name="Catch2Wshed">Catch2Wshed!$A$1:$O$309</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1262" uniqueCount="604">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1262" uniqueCount="605">
   <si>
     <t>WshedID</t>
   </si>
@@ -1843,6 +1843,9 @@
   <si>
     <t>Wshed</t>
   </si>
+  <si>
+    <t>BFQ95</t>
+  </si>
 </sst>
 </file>
 
@@ -4492,7 +4495,7 @@
   <dimension ref="A1:X309"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:O1048576"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4523,7 +4526,7 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>604</v>
       </c>
       <c r="H1" t="s">
         <v>6</v>
@@ -4591,7 +4594,7 @@
         <v>4563</v>
       </c>
       <c r="G2">
-        <v>75896200</v>
+        <v>4.0780000000000003</v>
       </c>
       <c r="H2">
         <v>345</v>
@@ -4667,7 +4670,7 @@
         <v>5383</v>
       </c>
       <c r="G3">
-        <v>57027200</v>
+        <v>2.1440000000000001</v>
       </c>
       <c r="H3">
         <v>1047</v>
@@ -4695,11 +4698,11 @@
       </c>
       <c r="Q3">
         <f>Catch2Wshed!$H$3*PRODUCT(Nodes!$K$50:$R$50)*PRODUCT(Nodes!$K$40:$R$40)</f>
-        <v>2094</v>
+        <v>65.4375</v>
       </c>
       <c r="R3">
         <f>Catch2Wshed!$I$3*PRODUCT(Nodes!$K$50:$S$50)*PRODUCT(Nodes!$K$40:$S$40)</f>
-        <v>864</v>
+        <v>27</v>
       </c>
       <c r="S3">
         <f>Catch2Wshed!$J$3*PRODUCT(Nodes!$K$50:$R$50)*PRODUCT(Nodes!$K$40:$R$40)</f>
@@ -4707,7 +4710,7 @@
       </c>
       <c r="T3">
         <f>Catch2Wshed!$K$3*PRODUCT(Nodes!$K$50:$R$50)*PRODUCT(Nodes!$K$40:$R$40)</f>
-        <v>2646</v>
+        <v>82.6875</v>
       </c>
       <c r="U3">
         <f>Catch2Wshed!$L$3*PRODUCT(Nodes!$K$50:$R$50)*PRODUCT(Nodes!$K$40:$R$40)</f>
@@ -4715,7 +4718,7 @@
       </c>
       <c r="V3">
         <f>Catch2Wshed!$M$3*PRODUCT(Nodes!$K$50:$R$50)*PRODUCT(Nodes!$K$40:$R$40)</f>
-        <v>792</v>
+        <v>24.75</v>
       </c>
       <c r="W3">
         <f>Catch2Wshed!$N$3*PRODUCT(Nodes!$K$50:$R$50)*PRODUCT(Nodes!$K$40:$R$40)</f>
@@ -4723,7 +4726,7 @@
       </c>
       <c r="X3">
         <f>Catch2Wshed!$O$3*PRODUCT(Nodes!$K$50:$R$50)*PRODUCT(Nodes!$K$40:$R$40)</f>
-        <v>626</v>
+        <v>19.5625</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
@@ -4743,7 +4746,7 @@
         <v>6742</v>
       </c>
       <c r="G4">
-        <v>73888200</v>
+        <v>0.74299999999999999</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -4819,7 +4822,7 @@
         <v>6383</v>
       </c>
       <c r="G5">
-        <v>211769000</v>
+        <v>1.5529999999999999</v>
       </c>
       <c r="H5">
         <v>1204</v>
@@ -4847,11 +4850,11 @@
       </c>
       <c r="Q5">
         <f>Catch2Wshed!$H$5*PRODUCT(Nodes!$K$197:$R$197)*PRODUCT(Nodes!$K$50:$R$50)*PRODUCT(Nodes!$K$40:$R$40)</f>
-        <v>202.27199999999999</v>
+        <v>6.3209999999999997</v>
       </c>
       <c r="R5">
         <f>Catch2Wshed!$I$5*PRODUCT(Nodes!$K$197:$R$197)*PRODUCT(Nodes!$K$50:$R$50)*PRODUCT(Nodes!$K$40:$R$40)</f>
-        <v>4.5359999999999996</v>
+        <v>0.14174999999999999</v>
       </c>
       <c r="S5">
         <f>Catch2Wshed!$J$5*PRODUCT(Nodes!$K$197:$R$197)*PRODUCT(Nodes!$K$50:$R$50)*PRODUCT(Nodes!$K$40:$R$40)</f>
@@ -4859,7 +4862,7 @@
       </c>
       <c r="T5">
         <f>Catch2Wshed!$K$5*PRODUCT(Nodes!$K$197:$R$197)*PRODUCT(Nodes!$K$50:$R$50)*PRODUCT(Nodes!$K$40:$R$40)</f>
-        <v>90.719999999999985</v>
+        <v>2.8349999999999995</v>
       </c>
       <c r="U5">
         <f>Catch2Wshed!$L$5*PRODUCT(Nodes!$K$197:$R$197)*PRODUCT(Nodes!$K$50:$R$50)*PRODUCT(Nodes!$K$40:$R$40)</f>
@@ -4867,7 +4870,7 @@
       </c>
       <c r="V5">
         <f>Catch2Wshed!$M$5*PRODUCT(Nodes!$K$197:$R$197)*PRODUCT(Nodes!$K$50:$R$50)*PRODUCT(Nodes!$K$40:$R$40)</f>
-        <v>3.6959999999999997</v>
+        <v>0.11549999999999999</v>
       </c>
       <c r="W5">
         <f>Catch2Wshed!$N$5*PRODUCT(Nodes!$K$197:$R$197)*PRODUCT(Nodes!$K$50:$R$50)*PRODUCT(Nodes!$K$40:$R$40)</f>
@@ -4875,7 +4878,7 @@
       </c>
       <c r="X5">
         <f>Catch2Wshed!$O$5*PRODUCT(Nodes!$K$197:$R$197)*PRODUCT(Nodes!$K$50:$R$50)*PRODUCT(Nodes!$K$40:$R$40)</f>
-        <v>3.3599999999999994</v>
+        <v>0.10499999999999998</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
@@ -4895,7 +4898,7 @@
         <v>4637</v>
       </c>
       <c r="G6">
-        <v>33375000</v>
+        <v>1.706</v>
       </c>
       <c r="H6">
         <v>445</v>
@@ -4971,7 +4974,7 @@
         <v>5735</v>
       </c>
       <c r="G7">
-        <v>37154500</v>
+        <v>0.70199999999999996</v>
       </c>
       <c r="H7">
         <v>308</v>
@@ -4999,11 +5002,11 @@
       </c>
       <c r="Q7">
         <f>Catch2Wshed!$H$7*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
-        <v>308</v>
+        <v>616</v>
       </c>
       <c r="R7">
         <f>Catch2Wshed!$I$7*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
-        <v>147</v>
+        <v>294</v>
       </c>
       <c r="S7">
         <f>Catch2Wshed!$J$7*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
@@ -5011,7 +5014,7 @@
       </c>
       <c r="T7">
         <f>Catch2Wshed!$K$7*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
-        <v>523</v>
+        <v>1046</v>
       </c>
       <c r="U7">
         <f>Catch2Wshed!$L$7*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
@@ -5019,7 +5022,7 @@
       </c>
       <c r="V7">
         <f>Catch2Wshed!$M$7*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
-        <v>126</v>
+        <v>252</v>
       </c>
       <c r="W7">
         <f>Catch2Wshed!$N$7*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
@@ -5027,7 +5030,7 @@
       </c>
       <c r="X7">
         <f>Catch2Wshed!$O$7*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
-        <v>78</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
@@ -5047,7 +5050,7 @@
         <v>5945</v>
       </c>
       <c r="G8">
-        <v>19819000</v>
+        <v>0.318</v>
       </c>
       <c r="H8">
         <v>300</v>
@@ -5075,11 +5078,11 @@
       </c>
       <c r="Q8">
         <f>Catch2Wshed!$H$8*PRODUCT(Nodes!$K$230:$R$230)*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
-        <v>11.34</v>
+        <v>22.68</v>
       </c>
       <c r="R8">
         <f>Catch2Wshed!$I$8*PRODUCT(Nodes!$K$230:$R$230)*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
-        <v>2.0790000000000002</v>
+        <v>4.1580000000000004</v>
       </c>
       <c r="S8">
         <f>Catch2Wshed!$J$8*PRODUCT(Nodes!$K$230:$R$230)*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
@@ -5087,7 +5090,7 @@
       </c>
       <c r="T8">
         <f>Catch2Wshed!$K$8*PRODUCT(Nodes!$K$230:$R$230)*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
-        <v>9.0342000000000002</v>
+        <v>18.0684</v>
       </c>
       <c r="U8">
         <f>Catch2Wshed!$L$8*PRODUCT(Nodes!$K$230:$R$230)*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
@@ -5095,7 +5098,7 @@
       </c>
       <c r="V8">
         <f>Catch2Wshed!$M$8*PRODUCT(Nodes!$K$230:$R$230)*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
-        <v>1.7387999999999999</v>
+        <v>3.4775999999999998</v>
       </c>
       <c r="W8">
         <f>Catch2Wshed!$N$8*PRODUCT(Nodes!$K$230:$R$230)*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
@@ -5103,7 +5106,7 @@
       </c>
       <c r="X8">
         <f>Catch2Wshed!$O$8*PRODUCT(Nodes!$K$230:$R$230)*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
-        <v>1.3608</v>
+        <v>2.7216</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
@@ -5123,7 +5126,7 @@
         <v>6176</v>
       </c>
       <c r="G9">
-        <v>5373120</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -5199,7 +5202,7 @@
         <v>5745</v>
       </c>
       <c r="G10">
-        <v>155319000</v>
+        <v>0.67800000000000005</v>
       </c>
       <c r="H10">
         <v>2380</v>
@@ -5227,11 +5230,11 @@
       </c>
       <c r="Q10">
         <f>Catch2Wshed!$H$10*PRODUCT(Nodes!$K$193:$R$193)*PRODUCT(Nodes!$K$230:$R$230)*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
-        <v>7.5569759999999997</v>
+        <v>15.113951999999999</v>
       </c>
       <c r="R10">
         <f>Catch2Wshed!$I$10*PRODUCT(Nodes!$K$193:$R$193)*PRODUCT(Nodes!$K$230:$R$230)*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
-        <v>0.11748239999999999</v>
+        <v>0.23496479999999997</v>
       </c>
       <c r="S10">
         <f>Catch2Wshed!$J$10*PRODUCT(Nodes!$K$193:$R$193)*PRODUCT(Nodes!$K$230:$R$230)*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
@@ -5239,7 +5242,7 @@
       </c>
       <c r="T10">
         <f>Catch2Wshed!$K$10*PRODUCT(Nodes!$K$193:$R$193)*PRODUCT(Nodes!$K$230:$R$230)*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
-        <v>2.4671303999999994</v>
+        <v>4.9342607999999988</v>
       </c>
       <c r="U10">
         <f>Catch2Wshed!$L$10*PRODUCT(Nodes!$K$193:$R$193)*PRODUCT(Nodes!$K$230:$R$230)*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
@@ -5247,7 +5250,7 @@
       </c>
       <c r="V10">
         <f>Catch2Wshed!$M$10*PRODUCT(Nodes!$K$193:$R$193)*PRODUCT(Nodes!$K$230:$R$230)*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
-        <v>7.9379999999999992E-2</v>
+        <v>0.15875999999999998</v>
       </c>
       <c r="W10">
         <f>Catch2Wshed!$N$10*PRODUCT(Nodes!$K$193:$R$193)*PRODUCT(Nodes!$K$230:$R$230)*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
@@ -5255,7 +5258,7 @@
       </c>
       <c r="X10">
         <f>Catch2Wshed!$O$10*PRODUCT(Nodes!$K$193:$R$193)*PRODUCT(Nodes!$K$230:$R$230)*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
-        <v>6.6679199999999994E-2</v>
+        <v>0.13335839999999999</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
@@ -5275,7 +5278,7 @@
         <v>4418</v>
       </c>
       <c r="G11">
-        <v>414272000</v>
+        <v>1.9259999999999999</v>
       </c>
       <c r="H11">
         <v>3557</v>
@@ -5303,11 +5306,11 @@
       </c>
       <c r="Q11">
         <f>Catch2Wshed!$H$11*PRODUCT(Nodes!$K$195:$R$195)*PRODUCT(Nodes!$K$230:$R$230)*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
-        <v>11.294186399999999</v>
+        <v>22.588372799999998</v>
       </c>
       <c r="R11">
         <f>Catch2Wshed!$I$11*PRODUCT(Nodes!$K$195:$R$195)*PRODUCT(Nodes!$K$230:$R$230)*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
-        <v>0.11430719999999998</v>
+        <v>0.22861439999999997</v>
       </c>
       <c r="S11">
         <f>Catch2Wshed!$J$11*PRODUCT(Nodes!$K$195:$R$195)*PRODUCT(Nodes!$K$230:$R$230)*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
@@ -5315,7 +5318,7 @@
       </c>
       <c r="T11">
         <f>Catch2Wshed!$K$11*PRODUCT(Nodes!$K$195:$R$195)*PRODUCT(Nodes!$K$230:$R$230)*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
-        <v>2.7306719999999998</v>
+        <v>5.4613439999999995</v>
       </c>
       <c r="U11">
         <f>Catch2Wshed!$L$11*PRODUCT(Nodes!$K$195:$R$195)*PRODUCT(Nodes!$K$230:$R$230)*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
@@ -5323,7 +5326,7 @@
       </c>
       <c r="V11">
         <f>Catch2Wshed!$M$11*PRODUCT(Nodes!$K$195:$R$195)*PRODUCT(Nodes!$K$230:$R$230)*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
-        <v>7.6204800000000003E-2</v>
+        <v>0.15240960000000001</v>
       </c>
       <c r="W11">
         <f>Catch2Wshed!$N$11*PRODUCT(Nodes!$K$195:$R$195)*PRODUCT(Nodes!$K$230:$R$230)*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
@@ -5331,7 +5334,7 @@
       </c>
       <c r="X11">
         <f>Catch2Wshed!$O$11*PRODUCT(Nodes!$K$195:$R$195)*PRODUCT(Nodes!$K$230:$R$230)*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
-        <v>6.3503999999999991E-2</v>
+        <v>0.12700799999999998</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
@@ -5351,7 +5354,7 @@
         <v>4908</v>
       </c>
       <c r="G12">
-        <v>36807600</v>
+        <v>1.4850000000000001</v>
       </c>
       <c r="H12">
         <v>502</v>
@@ -5427,7 +5430,7 @@
         <v>5595</v>
       </c>
       <c r="G13">
-        <v>5209330</v>
+        <v>5.5E-2</v>
       </c>
       <c r="H13">
         <v>99</v>
@@ -5455,11 +5458,11 @@
       </c>
       <c r="Q13">
         <f>Catch2Wshed!$H$13*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
-        <v>99</v>
+        <v>198</v>
       </c>
       <c r="R13">
         <f>Catch2Wshed!$I$13*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="S13">
         <f>Catch2Wshed!$J$13*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
@@ -5467,7 +5470,7 @@
       </c>
       <c r="T13">
         <f>Catch2Wshed!$K$13*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
-        <v>142</v>
+        <v>284</v>
       </c>
       <c r="U13">
         <f>Catch2Wshed!$L$13*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
@@ -5475,7 +5478,7 @@
       </c>
       <c r="V13">
         <f>Catch2Wshed!$M$13*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="W13">
         <f>Catch2Wshed!$N$13*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
@@ -5483,7 +5486,7 @@
       </c>
       <c r="X13">
         <f>Catch2Wshed!$O$13*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
-        <v>14</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
@@ -5503,7 +5506,7 @@
         <v>5679</v>
       </c>
       <c r="G14">
-        <v>3276570</v>
+        <v>2.7E-2</v>
       </c>
       <c r="H14">
         <v>181</v>
@@ -5531,11 +5534,11 @@
       </c>
       <c r="Q14">
         <f>Catch2Wshed!$H$14*PRODUCT(Nodes!$K$196:$R$196)*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
-        <v>15.203999999999999</v>
+        <v>30.407999999999998</v>
       </c>
       <c r="R14">
         <f>Catch2Wshed!$I$14*PRODUCT(Nodes!$K$196:$R$196)*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
-        <v>2.4359999999999999</v>
+        <v>4.8719999999999999</v>
       </c>
       <c r="S14">
         <f>Catch2Wshed!$J$14*PRODUCT(Nodes!$K$196:$R$196)*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
@@ -5543,7 +5546,7 @@
       </c>
       <c r="T14">
         <f>Catch2Wshed!$K$14*PRODUCT(Nodes!$K$196:$R$196)*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
-        <v>14.195999999999998</v>
+        <v>28.391999999999996</v>
       </c>
       <c r="U14">
         <f>Catch2Wshed!$L$14*PRODUCT(Nodes!$K$196:$R$196)*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
@@ -5551,7 +5554,7 @@
       </c>
       <c r="V14">
         <f>Catch2Wshed!$M$14*PRODUCT(Nodes!$K$196:$R$196)*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
-        <v>1.5959999999999999</v>
+        <v>3.1919999999999997</v>
       </c>
       <c r="W14">
         <f>Catch2Wshed!$N$14*PRODUCT(Nodes!$K$196:$R$196)*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
@@ -5559,7 +5562,7 @@
       </c>
       <c r="X14">
         <f>Catch2Wshed!$O$14*PRODUCT(Nodes!$K$196:$R$196)*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
-        <v>1.0919999999999999</v>
+        <v>2.1839999999999997</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
@@ -5579,7 +5582,7 @@
         <v>6084</v>
       </c>
       <c r="G15">
-        <v>11291800</v>
+        <v>0.11700000000000001</v>
       </c>
       <c r="H15">
         <v>5</v>
@@ -5607,11 +5610,11 @@
       </c>
       <c r="Q15">
         <f>Catch2Wshed!$H$15*PRODUCT(Nodes!$K$187:$R$187)*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
-        <v>0.41999999999999993</v>
+        <v>0.83999999999999986</v>
       </c>
       <c r="R15">
         <f>Catch2Wshed!$I$15*PRODUCT(Nodes!$K$187:$R$187)*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
-        <v>8.3999999999999991E-2</v>
+        <v>0.16799999999999998</v>
       </c>
       <c r="S15">
         <f>Catch2Wshed!$J$15*PRODUCT(Nodes!$K$187:$R$187)*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
@@ -5619,7 +5622,7 @@
       </c>
       <c r="T15">
         <f>Catch2Wshed!$K$15*PRODUCT(Nodes!$K$187:$R$187)*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
-        <v>0.33599999999999997</v>
+        <v>0.67199999999999993</v>
       </c>
       <c r="U15">
         <f>Catch2Wshed!$L$15*PRODUCT(Nodes!$K$187:$R$187)*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
@@ -5655,7 +5658,7 @@
         <v>6739</v>
       </c>
       <c r="G16">
-        <v>14422300</v>
+        <v>0.114</v>
       </c>
       <c r="H16">
         <v>0</v>
@@ -5731,7 +5734,7 @@
         <v>6747</v>
       </c>
       <c r="G17">
-        <v>47275900</v>
+        <v>0.55400000000000005</v>
       </c>
       <c r="H17">
         <v>1607</v>
@@ -5759,11 +5762,11 @@
       </c>
       <c r="Q17">
         <f>Catch2Wshed!$H$17*PRODUCT(Nodes!$K$189:$R$189)*PRODUCT(Nodes!$K$196:$R$196)*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
-        <v>11.338991999999999</v>
+        <v>22.677983999999999</v>
       </c>
       <c r="R17">
         <f>Catch2Wshed!$I$17*PRODUCT(Nodes!$K$189:$R$189)*PRODUCT(Nodes!$K$196:$R$196)*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
-        <v>0.23990399999999998</v>
+        <v>0.47980799999999996</v>
       </c>
       <c r="S17">
         <f>Catch2Wshed!$J$17*PRODUCT(Nodes!$K$189:$R$189)*PRODUCT(Nodes!$K$196:$R$196)*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
@@ -5771,7 +5774,7 @@
       </c>
       <c r="T17">
         <f>Catch2Wshed!$K$17*PRODUCT(Nodes!$K$189:$R$189)*PRODUCT(Nodes!$K$196:$R$196)*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
-        <v>6.1387199999999993</v>
+        <v>12.277439999999999</v>
       </c>
       <c r="U17">
         <f>Catch2Wshed!$L$17*PRODUCT(Nodes!$K$189:$R$189)*PRODUCT(Nodes!$K$196:$R$196)*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
@@ -5779,7 +5782,7 @@
       </c>
       <c r="V17">
         <f>Catch2Wshed!$M$17*PRODUCT(Nodes!$K$189:$R$189)*PRODUCT(Nodes!$K$196:$R$196)*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
-        <v>0.14111999999999997</v>
+        <v>0.28223999999999994</v>
       </c>
       <c r="W17">
         <f>Catch2Wshed!$N$17*PRODUCT(Nodes!$K$189:$R$189)*PRODUCT(Nodes!$K$196:$R$196)*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
@@ -5787,7 +5790,7 @@
       </c>
       <c r="X17">
         <f>Catch2Wshed!O$17*PRODUCT(Nodes!$K$189:$R$189)*PRODUCT(Nodes!$K$196:$R$196)*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
-        <v>8.4671999999999997E-2</v>
+        <v>0.16934399999999999</v>
       </c>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
@@ -5807,7 +5810,7 @@
         <v>5097</v>
       </c>
       <c r="G18">
-        <v>14654100</v>
+        <v>0.33100000000000002</v>
       </c>
       <c r="H18">
         <v>0</v>
@@ -5883,7 +5886,7 @@
         <v>5910</v>
       </c>
       <c r="G19">
-        <v>4503720</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -5959,7 +5962,7 @@
         <v>5111</v>
       </c>
       <c r="G20">
-        <v>33944800</v>
+        <v>1.1180000000000001</v>
       </c>
       <c r="H20">
         <v>750</v>
@@ -6035,7 +6038,7 @@
         <v>5492</v>
       </c>
       <c r="G21">
-        <v>2279230</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="H21">
         <v>0</v>
@@ -6111,7 +6114,7 @@
         <v>5909</v>
       </c>
       <c r="G22">
-        <v>3468330</v>
+        <v>2.4E-2</v>
       </c>
       <c r="H22">
         <v>0</v>
@@ -6187,7 +6190,7 @@
         <v>6435</v>
       </c>
       <c r="G23">
-        <v>12484800</v>
+        <v>0.105</v>
       </c>
       <c r="H23">
         <v>0</v>
@@ -6263,7 +6266,7 @@
         <v>6108</v>
       </c>
       <c r="G24">
-        <v>111538000</v>
+        <v>0.77200000000000002</v>
       </c>
       <c r="H24">
         <v>843</v>
@@ -6339,7 +6342,7 @@
         <v>5055</v>
       </c>
       <c r="G25">
-        <v>35654600</v>
+        <v>1.323</v>
       </c>
       <c r="H25">
         <v>706</v>
@@ -6415,7 +6418,7 @@
         <v>5636</v>
       </c>
       <c r="G26">
-        <v>1482320</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="H26">
         <v>0</v>
@@ -6491,7 +6494,7 @@
         <v>5521</v>
       </c>
       <c r="G27">
-        <v>1777660</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="H27">
         <v>0</v>
@@ -6567,7 +6570,7 @@
         <v>6031</v>
       </c>
       <c r="G28">
-        <v>10933800</v>
+        <v>0.128</v>
       </c>
       <c r="H28">
         <v>0</v>
@@ -6643,7 +6646,7 @@
         <v>6565</v>
       </c>
       <c r="G29">
-        <v>59996000</v>
+        <v>1.0620000000000001</v>
       </c>
       <c r="H29">
         <v>1668</v>
@@ -6719,7 +6722,7 @@
         <v>5053</v>
       </c>
       <c r="G30">
-        <v>60462500</v>
+        <v>2.6379999999999999</v>
       </c>
       <c r="H30">
         <v>1919</v>
@@ -6795,7 +6798,7 @@
         <v>5889</v>
       </c>
       <c r="G31">
-        <v>2962360</v>
+        <v>1.9E-2</v>
       </c>
       <c r="H31">
         <v>0</v>
@@ -6871,7 +6874,7 @@
         <v>5866</v>
       </c>
       <c r="G32">
-        <v>2557500</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="H32">
         <v>0</v>
@@ -6947,7 +6950,7 @@
         <v>5720</v>
       </c>
       <c r="G33">
-        <v>692101</v>
+        <v>2E-3</v>
       </c>
       <c r="H33">
         <v>36</v>
@@ -7023,7 +7026,7 @@
         <v>6435</v>
       </c>
       <c r="G34">
-        <v>47355900</v>
+        <v>0.53400000000000003</v>
       </c>
       <c r="H34">
         <v>1493</v>
@@ -7099,7 +7102,7 @@
         <v>3937</v>
       </c>
       <c r="G35">
-        <v>398375000</v>
+        <v>1.6859999999999999</v>
       </c>
       <c r="H35">
         <v>3395</v>
@@ -7175,7 +7178,7 @@
         <v>5095</v>
       </c>
       <c r="G36">
-        <v>52238700</v>
+        <v>1.518</v>
       </c>
       <c r="H36">
         <v>1072</v>
@@ -7251,7 +7254,7 @@
         <v>4199</v>
       </c>
       <c r="G37">
-        <v>385667000</v>
+        <v>1.54</v>
       </c>
       <c r="H37">
         <v>4660</v>
@@ -7327,7 +7330,7 @@
         <v>5015</v>
       </c>
       <c r="G38">
-        <v>49759700</v>
+        <v>1.9239999999999999</v>
       </c>
       <c r="H38">
         <v>1371</v>
@@ -7403,7 +7406,7 @@
         <v>3990</v>
       </c>
       <c r="G39">
-        <v>380969000</v>
+        <v>1.397</v>
       </c>
       <c r="H39">
         <v>3523</v>
@@ -7479,7 +7482,7 @@
         <v>4587</v>
       </c>
       <c r="G40">
-        <v>109540000</v>
+        <v>6.15</v>
       </c>
       <c r="H40">
         <v>1243</v>
@@ -7555,7 +7558,7 @@
         <v>5816</v>
       </c>
       <c r="G41">
-        <v>5018970</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="H41">
         <v>0</v>
@@ -7631,7 +7634,7 @@
         <v>5937</v>
       </c>
       <c r="G42">
-        <v>5610800</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="H42">
         <v>0</v>
@@ -7707,7 +7710,7 @@
         <v>5878</v>
       </c>
       <c r="G43">
-        <v>1363640</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="H43">
         <v>5</v>
@@ -7783,7 +7786,7 @@
         <v>6576</v>
       </c>
       <c r="G44">
-        <v>89005900</v>
+        <v>1.4370000000000001</v>
       </c>
       <c r="H44">
         <v>1887</v>
@@ -7859,7 +7862,7 @@
         <v>2683</v>
       </c>
       <c r="G45">
-        <v>254320000</v>
+        <v>0.72099999999999997</v>
       </c>
       <c r="H45">
         <v>2652</v>
@@ -7935,7 +7938,7 @@
         <v>4593</v>
       </c>
       <c r="G46">
-        <v>77894400</v>
+        <v>4.2329999999999997</v>
       </c>
       <c r="H46">
         <v>1005</v>
@@ -8011,7 +8014,7 @@
         <v>5550</v>
       </c>
       <c r="G47">
-        <v>33665400</v>
+        <v>0.94499999999999995</v>
       </c>
       <c r="H47">
         <v>677</v>
@@ -8039,11 +8042,11 @@
       </c>
       <c r="Q47">
         <f>Catch2Wshed!$H$47*PRODUCT(Nodes!$K$55:$R$55)*PRODUCT(Nodes!$K$35:$R$35)</f>
-        <v>1354</v>
+        <v>42.3125</v>
       </c>
       <c r="R47">
         <f>Catch2Wshed!$I$47*PRODUCT(Nodes!$K$55:$R$55)*PRODUCT(Nodes!$K$35:$R$35)</f>
-        <v>380</v>
+        <v>11.875</v>
       </c>
       <c r="S47">
         <f>Catch2Wshed!$J$47*PRODUCT(Nodes!$K$55:$R$55)*PRODUCT(Nodes!$K$35:$R$35)</f>
@@ -8051,7 +8054,7 @@
       </c>
       <c r="T47">
         <f>Catch2Wshed!$K$47*PRODUCT(Nodes!$K$55:$R$55)*PRODUCT(Nodes!$K$35:$R$35)</f>
-        <v>1714</v>
+        <v>53.5625</v>
       </c>
       <c r="U47">
         <f>Catch2Wshed!$L$47*PRODUCT(Nodes!$K$55:$R$55)*PRODUCT(Nodes!$K$35:$R$35)</f>
@@ -8059,7 +8062,7 @@
       </c>
       <c r="V47">
         <f>Catch2Wshed!$M$47*PRODUCT(Nodes!$K$55:$R$55)*PRODUCT(Nodes!$K$35:$R$35)</f>
-        <v>494</v>
+        <v>15.4375</v>
       </c>
       <c r="W47">
         <f>Catch2Wshed!$N$47*PRODUCT(Nodes!$K$55:$R$55)*PRODUCT(Nodes!$K$35:$R$35)</f>
@@ -8067,7 +8070,7 @@
       </c>
       <c r="X47">
         <f>Catch2Wshed!$O$47*PRODUCT(Nodes!$K$55:$R$55)*PRODUCT(Nodes!$K$35:$R$35)</f>
-        <v>216</v>
+        <v>6.75</v>
       </c>
     </row>
     <row r="48" spans="1:24" x14ac:dyDescent="0.25">
@@ -8087,7 +8090,7 @@
         <v>5696</v>
       </c>
       <c r="G48">
-        <v>1401210</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="H48">
         <v>0</v>
@@ -8163,7 +8166,7 @@
         <v>5863</v>
       </c>
       <c r="G49">
-        <v>4333070</v>
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="H49">
         <v>0</v>
@@ -8239,7 +8242,7 @@
         <v>5900</v>
       </c>
       <c r="G50">
-        <v>2413150</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="H50">
         <v>0</v>
@@ -8315,7 +8318,7 @@
         <v>5973</v>
       </c>
       <c r="G51">
-        <v>1672450</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="H51">
         <v>0</v>
@@ -8391,7 +8394,7 @@
         <v>5971</v>
       </c>
       <c r="G52">
-        <v>1498660</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="H52">
         <v>0</v>
@@ -8467,7 +8470,7 @@
         <v>6124</v>
       </c>
       <c r="G53">
-        <v>16541500</v>
+        <v>0.19</v>
       </c>
       <c r="H53">
         <v>0</v>
@@ -8543,7 +8546,7 @@
         <v>6270</v>
       </c>
       <c r="G54">
-        <v>14126300</v>
+        <v>0.13400000000000001</v>
       </c>
       <c r="H54">
         <v>0</v>
@@ -8619,7 +8622,7 @@
         <v>5142</v>
       </c>
       <c r="G55">
-        <v>196649000</v>
+        <v>0.90800000000000003</v>
       </c>
       <c r="H55">
         <v>2480</v>
@@ -8695,7 +8698,7 @@
         <v>4543</v>
       </c>
       <c r="G56">
-        <v>122881000</v>
+        <v>6.5309999999999997</v>
       </c>
       <c r="H56">
         <v>1961</v>
@@ -8771,7 +8774,7 @@
         <v>6256</v>
       </c>
       <c r="G57">
-        <v>224361000</v>
+        <v>6.0659999999999998</v>
       </c>
       <c r="H57">
         <v>1409</v>
@@ -8847,7 +8850,7 @@
         <v>4354</v>
       </c>
       <c r="G58">
-        <v>48438800</v>
+        <v>8.3699999999999992</v>
       </c>
       <c r="H58">
         <v>1543</v>
@@ -8923,7 +8926,7 @@
         <v>6355</v>
       </c>
       <c r="G59">
-        <v>111429000</v>
+        <v>2.9390000000000001</v>
       </c>
       <c r="H59">
         <v>2566</v>
@@ -8999,7 +9002,7 @@
         <v>6999</v>
       </c>
       <c r="G60">
-        <v>3268660</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="H60">
         <v>0</v>
@@ -9075,7 +9078,7 @@
         <v>6993</v>
       </c>
       <c r="G61">
-        <v>4244540</v>
+        <v>1.4E-2</v>
       </c>
       <c r="H61">
         <v>0</v>
@@ -9151,7 +9154,7 @@
         <v>6994</v>
       </c>
       <c r="G62">
-        <v>10652000</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="H62">
         <v>0</v>
@@ -9227,7 +9230,7 @@
         <v>6916</v>
       </c>
       <c r="G63">
-        <v>65463900</v>
+        <v>0.71899999999999997</v>
       </c>
       <c r="H63">
         <v>2683</v>
@@ -9303,7 +9306,7 @@
         <v>5893</v>
       </c>
       <c r="G64">
-        <v>179508000</v>
+        <v>0.97899999999999998</v>
       </c>
       <c r="H64">
         <v>2593</v>
@@ -9379,7 +9382,7 @@
         <v>3110</v>
       </c>
       <c r="G65">
-        <v>1129760000</v>
+        <v>7.0540000000000003</v>
       </c>
       <c r="H65">
         <v>9904</v>
@@ -9455,7 +9458,7 @@
         <v>4746</v>
       </c>
       <c r="G66">
-        <v>125230000</v>
+        <v>5.9180000000000001</v>
       </c>
       <c r="H66">
         <v>1613</v>
@@ -9531,7 +9534,7 @@
         <v>5737</v>
       </c>
       <c r="G67">
-        <v>831886</v>
+        <v>2E-3</v>
       </c>
       <c r="H67">
         <v>0</v>
@@ -9607,7 +9610,7 @@
         <v>5849</v>
       </c>
       <c r="G68">
-        <v>2427240</v>
+        <v>0.01</v>
       </c>
       <c r="H68">
         <v>0</v>
@@ -9683,7 +9686,7 @@
         <v>6227</v>
       </c>
       <c r="G69">
-        <v>2627590</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="H69">
         <v>0</v>
@@ -9759,7 +9762,7 @@
         <v>6069</v>
       </c>
       <c r="G70">
-        <v>6111750</v>
+        <v>0.04</v>
       </c>
       <c r="H70">
         <v>0</v>
@@ -9835,7 +9838,7 @@
         <v>6543</v>
       </c>
       <c r="G71">
-        <v>16618600</v>
+        <v>0.123</v>
       </c>
       <c r="H71">
         <v>839</v>
@@ -9911,7 +9914,7 @@
         <v>4984</v>
       </c>
       <c r="G72">
-        <v>138433000</v>
+        <v>5.4560000000000004</v>
       </c>
       <c r="H72">
         <v>2450</v>
@@ -9987,7 +9990,7 @@
         <v>5461</v>
       </c>
       <c r="G73">
-        <v>4308660</v>
+        <v>2.7E-2</v>
       </c>
       <c r="H73">
         <v>594</v>
@@ -10063,7 +10066,7 @@
         <v>6070</v>
       </c>
       <c r="G74">
-        <v>1304970</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="H74">
         <v>0</v>
@@ -10139,7 +10142,7 @@
         <v>6852</v>
       </c>
       <c r="G75">
-        <v>19692800</v>
+        <v>0.13200000000000001</v>
       </c>
       <c r="H75">
         <v>0</v>
@@ -10215,7 +10218,7 @@
         <v>6423</v>
       </c>
       <c r="G76">
-        <v>29983900</v>
+        <v>0.251</v>
       </c>
       <c r="H76">
         <v>1014</v>
@@ -10291,7 +10294,7 @@
         <v>6774</v>
       </c>
       <c r="G77">
-        <v>51683100</v>
+        <v>0.39</v>
       </c>
       <c r="H77">
         <v>1852</v>
@@ -10367,7 +10370,7 @@
         <v>6375</v>
       </c>
       <c r="G78">
-        <v>93849800</v>
+        <v>0.57199999999999995</v>
       </c>
       <c r="H78">
         <v>2474</v>
@@ -10443,7 +10446,7 @@
         <v>4144</v>
       </c>
       <c r="G79">
-        <v>329928000</v>
+        <v>1.2549999999999999</v>
       </c>
       <c r="H79">
         <v>2091</v>
@@ -10519,7 +10522,7 @@
         <v>4204</v>
       </c>
       <c r="G80">
-        <v>18504900</v>
+        <v>0.73799999999999999</v>
       </c>
       <c r="H80">
         <v>416</v>
@@ -10595,7 +10598,7 @@
         <v>4411</v>
       </c>
       <c r="G81">
-        <v>1071990</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="H81">
         <v>0</v>
@@ -10671,7 +10674,7 @@
         <v>4553</v>
       </c>
       <c r="G82">
-        <v>2722790</v>
+        <v>2.3E-2</v>
       </c>
       <c r="H82">
         <v>4</v>
@@ -10747,7 +10750,7 @@
         <v>4690</v>
       </c>
       <c r="G83">
-        <v>15891300</v>
+        <v>0.36599999999999999</v>
       </c>
       <c r="H83">
         <v>455</v>
@@ -10823,7 +10826,7 @@
         <v>4814</v>
       </c>
       <c r="G84">
-        <v>803989</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="H84">
         <v>0</v>
@@ -10899,7 +10902,7 @@
         <v>5111</v>
       </c>
       <c r="G85">
-        <v>13916100</v>
+        <v>0.16900000000000001</v>
       </c>
       <c r="H85">
         <v>0</v>
@@ -10975,7 +10978,7 @@
         <v>5264</v>
       </c>
       <c r="G86">
-        <v>15566400</v>
+        <v>0.19500000000000001</v>
       </c>
       <c r="H86">
         <v>542</v>
@@ -11051,7 +11054,7 @@
         <v>5559</v>
       </c>
       <c r="G87">
-        <v>1306320</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="H87">
         <v>0</v>
@@ -11127,7 +11130,7 @@
         <v>5838</v>
       </c>
       <c r="G88">
-        <v>2673690</v>
+        <v>0.01</v>
       </c>
       <c r="H88">
         <v>0</v>
@@ -11203,7 +11206,7 @@
         <v>5833</v>
       </c>
       <c r="G89">
-        <v>7308220</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="H89">
         <v>0</v>
@@ -11279,7 +11282,7 @@
         <v>6080</v>
       </c>
       <c r="G90">
-        <v>34946300</v>
+        <v>0.37</v>
       </c>
       <c r="H90">
         <v>1048</v>
@@ -11355,7 +11358,7 @@
         <v>3806</v>
       </c>
       <c r="G91">
-        <v>21429700</v>
+        <v>1.081</v>
       </c>
       <c r="H91">
         <v>1199</v>
@@ -11431,7 +11434,7 @@
         <v>4538</v>
       </c>
       <c r="G92">
-        <v>12525700</v>
+        <v>0.249</v>
       </c>
       <c r="H92">
         <v>980</v>
@@ -11507,7 +11510,7 @@
         <v>4911</v>
       </c>
       <c r="G93">
-        <v>8265900</v>
+        <v>9.2999999999999999E-2</v>
       </c>
       <c r="H93">
         <v>679</v>
@@ -11583,7 +11586,7 @@
         <v>5589</v>
       </c>
       <c r="G94">
-        <v>174137000</v>
+        <v>0.86099999999999999</v>
       </c>
       <c r="H94">
         <v>4217</v>
@@ -11659,7 +11662,7 @@
         <v>3870</v>
       </c>
       <c r="G95">
-        <v>27439200</v>
+        <v>1.5629999999999999</v>
       </c>
       <c r="H95">
         <v>707</v>
@@ -11735,7 +11738,7 @@
         <v>4445</v>
       </c>
       <c r="G96">
-        <v>12122100</v>
+        <v>0.20100000000000001</v>
       </c>
       <c r="H96">
         <v>0</v>
@@ -11811,7 +11814,7 @@
         <v>4550</v>
       </c>
       <c r="G97">
-        <v>1278600</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="H97">
         <v>0</v>
@@ -11887,7 +11890,7 @@
         <v>4747</v>
       </c>
       <c r="G98">
-        <v>7733500</v>
+        <v>7.9000000000000001E-2</v>
       </c>
       <c r="H98">
         <v>0</v>
@@ -11963,7 +11966,7 @@
         <v>4865</v>
       </c>
       <c r="G99">
-        <v>5361440</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="H99">
         <v>13</v>
@@ -12039,7 +12042,7 @@
         <v>4540</v>
       </c>
       <c r="G100">
-        <v>15835600</v>
+        <v>0.313</v>
       </c>
       <c r="H100">
         <v>815</v>
@@ -12115,7 +12118,7 @@
         <v>4758</v>
       </c>
       <c r="G101">
-        <v>1165750</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="H101">
         <v>0</v>
@@ -12191,7 +12194,7 @@
         <v>4777</v>
       </c>
       <c r="G102">
-        <v>458600</v>
+        <v>1E-3</v>
       </c>
       <c r="H102">
         <v>17</v>
@@ -12267,7 +12270,7 @@
         <v>5921</v>
       </c>
       <c r="G103">
-        <v>380163000</v>
+        <v>3.5529999999999999</v>
       </c>
       <c r="H103">
         <v>8974</v>
@@ -12343,7 +12346,7 @@
         <v>3762</v>
       </c>
       <c r="G104">
-        <v>29588900</v>
+        <v>1.349</v>
       </c>
       <c r="H104">
         <v>0</v>
@@ -12419,7 +12422,7 @@
         <v>4072</v>
       </c>
       <c r="G105">
-        <v>724738</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="H105">
         <v>0</v>
@@ -12495,7 +12498,7 @@
         <v>4198</v>
       </c>
       <c r="G106">
-        <v>1326600</v>
+        <v>0.01</v>
       </c>
       <c r="H106">
         <v>0</v>
@@ -12571,7 +12574,7 @@
         <v>4315</v>
       </c>
       <c r="G107">
-        <v>3611990</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="H107">
         <v>0</v>
@@ -12647,7 +12650,7 @@
         <v>4281</v>
       </c>
       <c r="G108">
-        <v>5214020</v>
+        <v>6.7000000000000004E-2</v>
       </c>
       <c r="H108">
         <v>0</v>
@@ -12723,7 +12726,7 @@
         <v>3565</v>
       </c>
       <c r="G109">
-        <v>11119100</v>
+        <v>0.45900000000000002</v>
       </c>
       <c r="H109">
         <v>332</v>
@@ -12799,7 +12802,7 @@
         <v>4302</v>
       </c>
       <c r="G110">
-        <v>18016300</v>
+        <v>0.45300000000000001</v>
       </c>
       <c r="H110">
         <v>801</v>
@@ -12875,7 +12878,7 @@
         <v>4562</v>
       </c>
       <c r="G111">
-        <v>1510180</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="H111">
         <v>0</v>
@@ -12951,7 +12954,7 @@
         <v>4698</v>
       </c>
       <c r="G112">
-        <v>5632480</v>
+        <v>4.7E-2</v>
       </c>
       <c r="H112">
         <v>0</v>
@@ -13027,7 +13030,7 @@
         <v>4543</v>
       </c>
       <c r="G113">
-        <v>308914</v>
+        <v>1E-3</v>
       </c>
       <c r="H113">
         <v>31</v>
@@ -13103,7 +13106,7 @@
         <v>4555</v>
       </c>
       <c r="G114">
-        <v>4568290</v>
+        <v>0.04</v>
       </c>
       <c r="H114">
         <v>253</v>
@@ -13179,7 +13182,7 @@
         <v>5444</v>
       </c>
       <c r="G115">
-        <v>66890100</v>
+        <v>1.1160000000000001</v>
       </c>
       <c r="H115">
         <v>1977</v>
@@ -13255,7 +13258,7 @@
         <v>3065</v>
       </c>
       <c r="G116">
-        <v>307744000</v>
+        <v>0.88800000000000001</v>
       </c>
       <c r="H116">
         <v>2893</v>
@@ -13331,7 +13334,7 @@
         <v>3424</v>
       </c>
       <c r="G117">
-        <v>16341400</v>
+        <v>0.96299999999999997</v>
       </c>
       <c r="H117">
         <v>297</v>
@@ -13407,7 +13410,7 @@
         <v>3823</v>
       </c>
       <c r="G118">
-        <v>1139160</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="H118">
         <v>0</v>
@@ -13483,7 +13486,7 @@
         <v>3891</v>
       </c>
       <c r="G119">
-        <v>1241070</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="H119">
         <v>4</v>
@@ -13559,7 +13562,7 @@
         <v>3861</v>
       </c>
       <c r="G120">
-        <v>857195</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="H120">
         <v>32</v>
@@ -13635,7 +13638,7 @@
         <v>4250</v>
       </c>
       <c r="G121">
-        <v>24332800</v>
+        <v>0.73699999999999999</v>
       </c>
       <c r="H121">
         <v>430</v>
@@ -13711,7 +13714,7 @@
         <v>4461</v>
       </c>
       <c r="G122">
-        <v>307819</v>
+        <v>1E-3</v>
       </c>
       <c r="H122">
         <v>0</v>
@@ -13787,7 +13790,7 @@
         <v>4526</v>
       </c>
       <c r="G123">
-        <v>995797</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="H123">
         <v>0</v>
@@ -13863,7 +13866,7 @@
         <v>4734</v>
       </c>
       <c r="G124">
-        <v>8421580</v>
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="H124">
         <v>0</v>
@@ -13939,7 +13942,7 @@
         <v>4698</v>
       </c>
       <c r="G125">
-        <v>12660800</v>
+        <v>0.14299999999999999</v>
       </c>
       <c r="H125">
         <v>0</v>
@@ -14015,7 +14018,7 @@
         <v>4628</v>
       </c>
       <c r="G126">
-        <v>277691</v>
+        <v>0</v>
       </c>
       <c r="H126">
         <v>0</v>
@@ -14091,7 +14094,7 @@
         <v>3234</v>
       </c>
       <c r="G127">
-        <v>6341830</v>
+        <v>0.223</v>
       </c>
       <c r="H127">
         <v>0</v>
@@ -14167,7 +14170,7 @@
         <v>3911</v>
       </c>
       <c r="G128">
-        <v>12522900</v>
+        <v>0.34300000000000003</v>
       </c>
       <c r="H128">
         <v>0</v>
@@ -14243,7 +14246,7 @@
         <v>3236</v>
       </c>
       <c r="G129">
-        <v>8170630</v>
+        <v>0.34100000000000003</v>
       </c>
       <c r="H129">
         <v>383</v>
@@ -14319,7 +14322,7 @@
         <v>3878</v>
       </c>
       <c r="G130">
-        <v>6541780</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="H130">
         <v>366</v>
@@ -14395,7 +14398,7 @@
         <v>4285</v>
       </c>
       <c r="G131">
-        <v>8162170</v>
+        <v>0.127</v>
       </c>
       <c r="H131">
         <v>452</v>
@@ -14471,7 +14474,7 @@
         <v>4479</v>
       </c>
       <c r="G132">
-        <v>506133</v>
+        <v>1E-3</v>
       </c>
       <c r="H132">
         <v>61</v>
@@ -14547,7 +14550,7 @@
         <v>5596</v>
       </c>
       <c r="G133">
-        <v>116840000</v>
+        <v>0.96799999999999997</v>
       </c>
       <c r="H133">
         <v>3125</v>
@@ -14623,7 +14626,7 @@
         <v>3325</v>
       </c>
       <c r="G134">
-        <v>25329800</v>
+        <v>1.5780000000000001</v>
       </c>
       <c r="H134">
         <v>662</v>
@@ -14699,7 +14702,7 @@
         <v>3580</v>
       </c>
       <c r="G135">
-        <v>175398</v>
+        <v>1E-3</v>
       </c>
       <c r="H135">
         <v>0</v>
@@ -14775,7 +14778,7 @@
         <v>3709</v>
       </c>
       <c r="G136">
-        <v>2129220</v>
+        <v>2.7E-2</v>
       </c>
       <c r="H136">
         <v>0</v>
@@ -14851,7 +14854,7 @@
         <v>3769</v>
       </c>
       <c r="G137">
-        <v>4409720</v>
+        <v>9.2999999999999999E-2</v>
       </c>
       <c r="H137">
         <v>286</v>
@@ -14927,7 +14930,7 @@
         <v>3882</v>
       </c>
       <c r="G138">
-        <v>2647360</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="H138">
         <v>149</v>
@@ -15003,7 +15006,7 @@
         <v>3973</v>
       </c>
       <c r="G139">
-        <v>516546</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="H139">
         <v>23</v>
@@ -15079,7 +15082,7 @@
         <v>4179</v>
       </c>
       <c r="G140">
-        <v>11246800</v>
+        <v>0.216</v>
       </c>
       <c r="H140">
         <v>370</v>
@@ -15155,7 +15158,7 @@
         <v>4227</v>
       </c>
       <c r="G141">
-        <v>9683150</v>
+        <v>0.16600000000000001</v>
       </c>
       <c r="H141">
         <v>635</v>
@@ -15231,7 +15234,7 @@
         <v>4398</v>
       </c>
       <c r="G142">
-        <v>1684310</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="H142">
         <v>0</v>
@@ -15307,7 +15310,7 @@
         <v>4449</v>
       </c>
       <c r="G143">
-        <v>2393440</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="H143">
         <v>0</v>
@@ -15383,7 +15386,7 @@
         <v>4378</v>
       </c>
       <c r="G144">
-        <v>271462</v>
+        <v>1E-3</v>
       </c>
       <c r="H144">
         <v>0</v>
@@ -15459,7 +15462,7 @@
         <v>4367</v>
       </c>
       <c r="G145">
-        <v>397361</v>
+        <v>1E-3</v>
       </c>
       <c r="H145">
         <v>0</v>
@@ -15535,7 +15538,7 @@
         <v>4334</v>
       </c>
       <c r="G146">
-        <v>619789</v>
+        <v>2E-3</v>
       </c>
       <c r="H146">
         <v>0</v>
@@ -15611,7 +15614,7 @@
         <v>4594</v>
       </c>
       <c r="G147">
-        <v>10700100</v>
+        <v>0.122</v>
       </c>
       <c r="H147">
         <v>0</v>
@@ -15687,7 +15690,7 @@
         <v>4700</v>
       </c>
       <c r="G148">
-        <v>9859950</v>
+        <v>8.8999999999999996E-2</v>
       </c>
       <c r="H148">
         <v>0</v>
@@ -15763,7 +15766,7 @@
         <v>4616</v>
       </c>
       <c r="G149">
-        <v>3867930</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="H149">
         <v>0</v>
@@ -15839,7 +15842,7 @@
         <v>4846</v>
       </c>
       <c r="G150">
-        <v>29621700</v>
+        <v>0.44600000000000001</v>
       </c>
       <c r="H150">
         <v>2218</v>
@@ -15915,7 +15918,7 @@
         <v>3091</v>
       </c>
       <c r="G151">
-        <v>20196800</v>
+        <v>1.5029999999999999</v>
       </c>
       <c r="H151">
         <v>0</v>
@@ -15991,7 +15994,7 @@
         <v>3428</v>
       </c>
       <c r="G152">
-        <v>298216</v>
+        <v>2E-3</v>
       </c>
       <c r="H152">
         <v>0</v>
@@ -16067,7 +16070,7 @@
         <v>3875</v>
       </c>
       <c r="G153">
-        <v>10955600</v>
+        <v>0.20399999999999999</v>
       </c>
       <c r="H153">
         <v>0</v>
@@ -16143,7 +16146,7 @@
         <v>4086</v>
       </c>
       <c r="G154">
-        <v>5846520</v>
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="H154">
         <v>0</v>
@@ -16219,7 +16222,7 @@
         <v>3955</v>
       </c>
       <c r="G155">
-        <v>435044</v>
+        <v>2E-3</v>
       </c>
       <c r="H155">
         <v>0</v>
@@ -16295,7 +16298,7 @@
         <v>4292</v>
       </c>
       <c r="G156">
-        <v>1236080</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="H156">
         <v>0</v>
@@ -16371,7 +16374,7 @@
         <v>4528</v>
       </c>
       <c r="G157">
-        <v>5890420</v>
+        <v>0.05</v>
       </c>
       <c r="H157">
         <v>0</v>
@@ -16447,7 +16450,7 @@
         <v>2958</v>
       </c>
       <c r="G158">
-        <v>16804500</v>
+        <v>0.97799999999999998</v>
       </c>
       <c r="H158">
         <v>717</v>
@@ -16523,7 +16526,7 @@
         <v>3412</v>
       </c>
       <c r="G159">
-        <v>2378230</v>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="H159">
         <v>74</v>
@@ -16599,7 +16602,7 @@
         <v>3812</v>
       </c>
       <c r="G160">
-        <v>31989000</v>
+        <v>1.0740000000000001</v>
       </c>
       <c r="H160">
         <v>904</v>
@@ -16675,7 +16678,7 @@
         <v>4322</v>
       </c>
       <c r="G161">
-        <v>13243800</v>
+        <v>0.20699999999999999</v>
       </c>
       <c r="H161">
         <v>507</v>
@@ -16751,7 +16754,7 @@
         <v>4396</v>
       </c>
       <c r="G162">
-        <v>505555</v>
+        <v>1E-3</v>
       </c>
       <c r="H162">
         <v>34</v>
@@ -16827,7 +16830,7 @@
         <v>3996</v>
       </c>
       <c r="G163">
-        <v>23243000</v>
+        <v>0.71199999999999997</v>
       </c>
       <c r="H163">
         <v>0</v>
@@ -16903,7 +16906,7 @@
         <v>4335</v>
       </c>
       <c r="G164">
-        <v>1049180</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="H164">
         <v>0</v>
@@ -16979,7 +16982,7 @@
         <v>4326</v>
       </c>
       <c r="G165">
-        <v>1319410</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="H165">
         <v>0</v>
@@ -17055,7 +17058,7 @@
         <v>4422</v>
       </c>
       <c r="G166">
-        <v>1684660</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="H166">
         <v>0</v>
@@ -17131,7 +17134,7 @@
         <v>4458</v>
       </c>
       <c r="G167">
-        <v>3352510</v>
+        <v>2.3E-2</v>
       </c>
       <c r="H167">
         <v>0</v>
@@ -17207,7 +17210,7 @@
         <v>5555</v>
       </c>
       <c r="G168">
-        <v>329763000</v>
+        <v>6.5449999999999999</v>
       </c>
       <c r="H168">
         <v>12327</v>
@@ -17283,7 +17286,7 @@
         <v>2821</v>
       </c>
       <c r="G169">
-        <v>8479260</v>
+        <v>0.502</v>
       </c>
       <c r="H169">
         <v>575</v>
@@ -17359,7 +17362,7 @@
         <v>3067</v>
       </c>
       <c r="G170">
-        <v>355748</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="H170">
         <v>33</v>
@@ -17435,7 +17438,7 @@
         <v>3193</v>
       </c>
       <c r="G171">
-        <v>3294960</v>
+        <v>8.5999999999999993E-2</v>
       </c>
       <c r="H171">
         <v>149</v>
@@ -17511,7 +17514,7 @@
         <v>3781</v>
       </c>
       <c r="G172">
-        <v>30140800</v>
+        <v>1.1180000000000001</v>
       </c>
       <c r="H172">
         <v>1107</v>
@@ -17587,7 +17590,7 @@
         <v>4334</v>
       </c>
       <c r="G173">
-        <v>1924340</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="H173">
         <v>90</v>
@@ -17663,7 +17666,7 @@
         <v>4319</v>
       </c>
       <c r="G174">
-        <v>1079770</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="H174">
         <v>133</v>
@@ -17739,7 +17742,7 @@
         <v>5184</v>
       </c>
       <c r="G175">
-        <v>135783000</v>
+        <v>1.86</v>
       </c>
       <c r="H175">
         <v>1280</v>
@@ -17815,7 +17818,7 @@
         <v>4353</v>
       </c>
       <c r="G176">
-        <v>407511000</v>
+        <v>2.6309999999999998</v>
       </c>
       <c r="H176">
         <v>5096</v>
@@ -17891,7 +17894,7 @@
         <v>2910</v>
       </c>
       <c r="G177">
-        <v>19878600</v>
+        <v>1.167</v>
       </c>
       <c r="H177">
         <v>103</v>
@@ -17967,7 +17970,7 @@
         <v>3684</v>
       </c>
       <c r="G178">
-        <v>21325500</v>
+        <v>0.64800000000000002</v>
       </c>
       <c r="H178">
         <v>0</v>
@@ -18043,7 +18046,7 @@
         <v>4294</v>
       </c>
       <c r="G179">
-        <v>9254110</v>
+        <v>0.123</v>
       </c>
       <c r="H179">
         <v>0</v>
@@ -18119,7 +18122,7 @@
         <v>2577</v>
       </c>
       <c r="G180">
-        <v>5985450</v>
+        <v>0.44500000000000001</v>
       </c>
       <c r="H180">
         <v>130</v>
@@ -18195,7 +18198,7 @@
         <v>2922</v>
       </c>
       <c r="G181">
-        <v>7677970</v>
+        <v>0.33700000000000002</v>
       </c>
       <c r="H181">
         <v>239</v>
@@ -18271,7 +18274,7 @@
         <v>3678</v>
       </c>
       <c r="G182">
-        <v>31741000</v>
+        <v>1.151</v>
       </c>
       <c r="H182">
         <v>952</v>
@@ -18347,7 +18350,7 @@
         <v>4081</v>
       </c>
       <c r="G183">
-        <v>318282</v>
+        <v>1E-3</v>
       </c>
       <c r="H183">
         <v>0</v>
@@ -18423,7 +18426,7 @@
         <v>4137</v>
       </c>
       <c r="G184">
-        <v>757145</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="H184">
         <v>0</v>
@@ -18499,7 +18502,7 @@
         <v>4248</v>
       </c>
       <c r="G185">
-        <v>6674200</v>
+        <v>6.6000000000000003E-2</v>
       </c>
       <c r="H185">
         <v>0</v>
@@ -18575,7 +18578,7 @@
         <v>4223</v>
       </c>
       <c r="G186">
-        <v>962906</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="H186">
         <v>0</v>
@@ -18651,7 +18654,7 @@
         <v>4280</v>
       </c>
       <c r="G187">
-        <v>2080240</v>
+        <v>0.01</v>
       </c>
       <c r="H187">
         <v>0</v>
@@ -18727,7 +18730,7 @@
         <v>4218</v>
       </c>
       <c r="G188">
-        <v>2113200</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="H188">
         <v>0</v>
@@ -18803,7 +18806,7 @@
         <v>4704</v>
       </c>
       <c r="G189">
-        <v>58067000</v>
+        <v>1.137</v>
       </c>
       <c r="H189">
         <v>0</v>
@@ -18879,7 +18882,7 @@
         <v>2545</v>
       </c>
       <c r="G190">
-        <v>17280400</v>
+        <v>1.75</v>
       </c>
       <c r="H190">
         <v>553</v>
@@ -18955,7 +18958,7 @@
         <v>2820</v>
       </c>
       <c r="G191">
-        <v>4114500</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="H191">
         <v>212</v>
@@ -19031,7 +19034,7 @@
         <v>3010</v>
       </c>
       <c r="G192">
-        <v>1498960</v>
+        <v>0.02</v>
       </c>
       <c r="H192">
         <v>3</v>
@@ -19107,7 +19110,7 @@
         <v>3567</v>
       </c>
       <c r="G193">
-        <v>19162600</v>
+        <v>0.437</v>
       </c>
       <c r="H193">
         <v>400</v>
@@ -19183,7 +19186,7 @@
         <v>3954</v>
       </c>
       <c r="G194">
-        <v>1296870</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="H194">
         <v>0</v>
@@ -19259,7 +19262,7 @@
         <v>2920</v>
       </c>
       <c r="G195">
-        <v>9765380</v>
+        <v>0.502</v>
       </c>
       <c r="H195">
         <v>386</v>
@@ -19335,7 +19338,7 @@
         <v>3088</v>
       </c>
       <c r="G196">
-        <v>617613</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="H196">
         <v>0</v>
@@ -19411,7 +19414,7 @@
         <v>3101</v>
       </c>
       <c r="G197">
-        <v>753596</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="H197">
         <v>0</v>
@@ -19487,7 +19490,7 @@
         <v>3311</v>
       </c>
       <c r="G198">
-        <v>6137930</v>
+        <v>0.11899999999999999</v>
       </c>
       <c r="H198">
         <v>377</v>
@@ -19563,7 +19566,7 @@
         <v>3589</v>
       </c>
       <c r="G199">
-        <v>11136400</v>
+        <v>0.21299999999999999</v>
       </c>
       <c r="H199">
         <v>0</v>
@@ -19639,7 +19642,7 @@
         <v>3949</v>
       </c>
       <c r="G200">
-        <v>2160190</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="H200">
         <v>0</v>
@@ -19715,7 +19718,7 @@
         <v>3522</v>
       </c>
       <c r="G201">
-        <v>15136900</v>
+        <v>0.36599999999999999</v>
       </c>
       <c r="H201">
         <v>729</v>
@@ -19791,7 +19794,7 @@
         <v>4008</v>
       </c>
       <c r="G202">
-        <v>448843</v>
+        <v>1E-3</v>
       </c>
       <c r="H202">
         <v>43</v>
@@ -19867,7 +19870,7 @@
         <v>4687</v>
       </c>
       <c r="G203">
-        <v>43701800</v>
+        <v>0.66800000000000004</v>
       </c>
       <c r="H203">
         <v>357</v>
@@ -19943,7 +19946,7 @@
         <v>2395</v>
       </c>
       <c r="G204">
-        <v>20138600</v>
+        <v>2.1779999999999999</v>
       </c>
       <c r="H204">
         <v>0</v>
@@ -20019,7 +20022,7 @@
         <v>2341</v>
       </c>
       <c r="G205">
-        <v>7867010</v>
+        <v>0.71</v>
       </c>
       <c r="H205">
         <v>151</v>
@@ -20095,7 +20098,7 @@
         <v>2748</v>
       </c>
       <c r="G206">
-        <v>7812280</v>
+        <v>0.38400000000000001</v>
       </c>
       <c r="H206">
         <v>160</v>
@@ -20245,7 +20248,7 @@
         <v>3026</v>
       </c>
       <c r="G208">
-        <v>4753600</v>
+        <v>0.125</v>
       </c>
       <c r="H208">
         <v>0</v>
@@ -20321,7 +20324,7 @@
         <v>3430</v>
       </c>
       <c r="G209">
-        <v>18822100</v>
+        <v>0.54300000000000004</v>
       </c>
       <c r="H209">
         <v>474</v>
@@ -20397,7 +20400,7 @@
         <v>3996</v>
       </c>
       <c r="G210">
-        <v>79921</v>
+        <v>0</v>
       </c>
       <c r="H210">
         <v>7</v>
@@ -20473,7 +20476,7 @@
         <v>4227</v>
       </c>
       <c r="G211">
-        <v>8500140</v>
+        <v>9.2999999999999999E-2</v>
       </c>
       <c r="H211">
         <v>205</v>
@@ -20549,7 +20552,7 @@
         <v>2218</v>
       </c>
       <c r="G212">
-        <v>14770500</v>
+        <v>1.2</v>
       </c>
       <c r="H212">
         <v>0</v>
@@ -20625,7 +20628,7 @@
         <v>2637</v>
       </c>
       <c r="G213">
-        <v>11502700</v>
+        <v>0.79300000000000004</v>
       </c>
       <c r="H213">
         <v>0</v>
@@ -20701,7 +20704,7 @@
         <v>2893</v>
       </c>
       <c r="G214">
-        <v>1145740</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="H214">
         <v>0</v>
@@ -20777,7 +20780,7 @@
         <v>2975</v>
       </c>
       <c r="G215">
-        <v>4682080</v>
+        <v>0.129</v>
       </c>
       <c r="H215">
         <v>0</v>
@@ -20853,7 +20856,7 @@
         <v>2047</v>
       </c>
       <c r="G216">
-        <v>20576600</v>
+        <v>2.2559999999999998</v>
       </c>
       <c r="H216">
         <v>0</v>
@@ -20929,7 +20932,7 @@
         <v>2023</v>
       </c>
       <c r="G217">
-        <v>22196800</v>
+        <v>3.9929999999999999</v>
       </c>
       <c r="H217">
         <v>427</v>
@@ -21005,7 +21008,7 @@
         <v>2613</v>
       </c>
       <c r="G218">
-        <v>14062600</v>
+        <v>1.0589999999999999</v>
       </c>
       <c r="H218">
         <v>603</v>
@@ -21081,7 +21084,7 @@
         <v>2915</v>
       </c>
       <c r="G219">
-        <v>2367380</v>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="H219">
         <v>0</v>
@@ -21157,7 +21160,7 @@
         <v>3251</v>
       </c>
       <c r="G220">
-        <v>11762000</v>
+        <v>0.31</v>
       </c>
       <c r="H220">
         <v>0</v>
@@ -21233,7 +21236,7 @@
         <v>2911</v>
       </c>
       <c r="G221">
-        <v>1103390</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="H221">
         <v>56</v>
@@ -21309,7 +21312,7 @@
         <v>3473</v>
       </c>
       <c r="G222">
-        <v>21347300</v>
+        <v>0.66900000000000004</v>
       </c>
       <c r="H222">
         <v>852</v>
@@ -21385,7 +21388,7 @@
         <v>3503</v>
       </c>
       <c r="G223">
-        <v>35788200</v>
+        <v>1.3640000000000001</v>
       </c>
       <c r="H223">
         <v>1174</v>
@@ -21461,7 +21464,7 @@
         <v>3981</v>
       </c>
       <c r="G224">
-        <v>680779</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="H224">
         <v>0</v>
@@ -21537,7 +21540,7 @@
         <v>4026</v>
       </c>
       <c r="G225">
-        <v>2496220</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="H225">
         <v>159</v>
@@ -21613,7 +21616,7 @@
         <v>4036</v>
       </c>
       <c r="G226">
-        <v>411638</v>
+        <v>1E-3</v>
       </c>
       <c r="H226">
         <v>0</v>
@@ -21689,7 +21692,7 @@
         <v>4056</v>
       </c>
       <c r="G227">
-        <v>1642510</v>
+        <v>0.01</v>
       </c>
       <c r="H227">
         <v>35</v>
@@ -21765,7 +21768,7 @@
         <v>4246</v>
       </c>
       <c r="G228">
-        <v>8395140</v>
+        <v>9.0999999999999998E-2</v>
       </c>
       <c r="H228">
         <v>0</v>
@@ -21841,7 +21844,7 @@
         <v>4724</v>
       </c>
       <c r="G229">
-        <v>72095100</v>
+        <v>1.367</v>
       </c>
       <c r="H229">
         <v>1126</v>
@@ -21917,7 +21920,7 @@
         <v>4875</v>
       </c>
       <c r="G230">
-        <v>176829000</v>
+        <v>2.7229999999999999</v>
       </c>
       <c r="H230">
         <v>3227</v>
@@ -21993,7 +21996,7 @@
         <v>2016</v>
       </c>
       <c r="G231">
-        <v>41604500</v>
+        <v>6.5410000000000004</v>
       </c>
       <c r="H231">
         <v>896</v>
@@ -22069,7 +22072,7 @@
         <v>2479</v>
       </c>
       <c r="G232">
-        <v>7926270</v>
+        <v>0.5</v>
       </c>
       <c r="H232">
         <v>214</v>
@@ -22145,7 +22148,7 @@
         <v>2769</v>
       </c>
       <c r="G233">
-        <v>2788060</v>
+        <v>6.2E-2</v>
       </c>
       <c r="H233">
         <v>0</v>
@@ -22221,7 +22224,7 @@
         <v>2859</v>
       </c>
       <c r="G234">
-        <v>5372490</v>
+        <v>0.158</v>
       </c>
       <c r="H234">
         <v>0</v>
@@ -22297,7 +22300,7 @@
         <v>3374</v>
       </c>
       <c r="G235">
-        <v>61044400</v>
+        <v>3.1019999999999999</v>
       </c>
       <c r="H235">
         <v>1210</v>
@@ -22373,7 +22376,7 @@
         <v>3916</v>
       </c>
       <c r="G236">
-        <v>1241360</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="H236">
         <v>0</v>
@@ -22449,7 +22452,7 @@
         <v>3975</v>
       </c>
       <c r="G237">
-        <v>536644</v>
+        <v>2E-3</v>
       </c>
       <c r="H237">
         <v>32</v>
@@ -22525,7 +22528,7 @@
         <v>4139</v>
       </c>
       <c r="G238">
-        <v>4474480</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="H238">
         <v>0</v>
@@ -22601,7 +22604,7 @@
         <v>4479</v>
       </c>
       <c r="G239">
-        <v>78805100</v>
+        <v>1.7509999999999999</v>
       </c>
       <c r="H239">
         <v>2036</v>
@@ -22677,7 +22680,7 @@
         <v>1876</v>
       </c>
       <c r="G240">
-        <v>3004560</v>
+        <v>0.45800000000000002</v>
       </c>
       <c r="H240">
         <v>0</v>
@@ -22753,7 +22756,7 @@
         <v>2243</v>
       </c>
       <c r="G241">
-        <v>28344700</v>
+        <v>2.7770000000000001</v>
       </c>
       <c r="H241">
         <v>669</v>
@@ -22829,7 +22832,7 @@
         <v>2774</v>
       </c>
       <c r="G242">
-        <v>5761400</v>
+        <v>0.13700000000000001</v>
       </c>
       <c r="H242">
         <v>0</v>
@@ -22905,7 +22908,7 @@
         <v>3135</v>
       </c>
       <c r="G243">
-        <v>39864000</v>
+        <v>1.758</v>
       </c>
       <c r="H243">
         <v>3036</v>
@@ -22981,7 +22984,7 @@
         <v>2791</v>
       </c>
       <c r="G244">
-        <v>4803980</v>
+        <v>0.14199999999999999</v>
       </c>
       <c r="H244">
         <v>0</v>
@@ -23057,7 +23060,7 @@
         <v>2686</v>
       </c>
       <c r="G245">
-        <v>639305</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="H245">
         <v>0</v>
@@ -23133,7 +23136,7 @@
         <v>3165</v>
       </c>
       <c r="G246">
-        <v>40062700</v>
+        <v>1.9339999999999999</v>
       </c>
       <c r="H246">
         <v>2370</v>
@@ -23209,7 +23212,7 @@
         <v>3304</v>
       </c>
       <c r="G247">
-        <v>28319700</v>
+        <v>1</v>
       </c>
       <c r="H247">
         <v>2508</v>
@@ -23285,7 +23288,7 @@
         <v>2040</v>
       </c>
       <c r="G248">
-        <v>9473570</v>
+        <v>0.85599999999999998</v>
       </c>
       <c r="H248">
         <v>942</v>
@@ -23361,7 +23364,7 @@
         <v>2359</v>
       </c>
       <c r="G249">
-        <v>7512400</v>
+        <v>0.45400000000000001</v>
       </c>
       <c r="H249">
         <v>334</v>
@@ -23437,7 +23440,7 @@
         <v>2272</v>
       </c>
       <c r="G250">
-        <v>4962170</v>
+        <v>0.23</v>
       </c>
       <c r="H250">
         <v>353</v>
@@ -23513,7 +23516,7 @@
         <v>2619</v>
       </c>
       <c r="G251">
-        <v>2281000</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="H251">
         <v>0</v>
@@ -23589,7 +23592,7 @@
         <v>2670</v>
       </c>
       <c r="G252">
-        <v>5151170</v>
+        <v>0.155</v>
       </c>
       <c r="H252">
         <v>329</v>
@@ -23665,7 +23668,7 @@
         <v>2636</v>
       </c>
       <c r="G253">
-        <v>2775630</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="H253">
         <v>164</v>
@@ -23741,7 +23744,7 @@
         <v>3331</v>
       </c>
       <c r="G254">
-        <v>39907100</v>
+        <v>1.667</v>
       </c>
       <c r="H254">
         <v>2061</v>
@@ -23817,7 +23820,7 @@
         <v>3947</v>
       </c>
       <c r="G255">
-        <v>2217970</v>
+        <v>1.4E-2</v>
       </c>
       <c r="H255">
         <v>0</v>
@@ -23893,7 +23896,7 @@
         <v>3905</v>
       </c>
       <c r="G256">
-        <v>4713500</v>
+        <v>0.04</v>
       </c>
       <c r="H256">
         <v>624</v>
@@ -23969,7 +23972,7 @@
         <v>3884</v>
       </c>
       <c r="G257">
-        <v>3522860</v>
+        <v>2.7E-2</v>
       </c>
       <c r="H257">
         <v>95</v>
@@ -24045,7 +24048,7 @@
         <v>3872</v>
       </c>
       <c r="G258">
-        <v>340743</v>
+        <v>1E-3</v>
       </c>
       <c r="H258">
         <v>47</v>
@@ -24121,7 +24124,7 @@
         <v>3685</v>
       </c>
       <c r="G259">
-        <v>2302880</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="H259">
         <v>243</v>
@@ -24197,7 +24200,7 @@
         <v>3850</v>
       </c>
       <c r="G260">
-        <v>4022790</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="H260">
         <v>574</v>
@@ -24273,7 +24276,7 @@
         <v>3792</v>
       </c>
       <c r="G261">
-        <v>8618400</v>
+        <v>0.11899999999999999</v>
       </c>
       <c r="H261">
         <v>734</v>
@@ -24349,7 +24352,7 @@
         <v>3346</v>
       </c>
       <c r="G262">
-        <v>1127470</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="H262">
         <v>0</v>
@@ -24425,7 +24428,7 @@
         <v>3388</v>
       </c>
       <c r="G263">
-        <v>2537590</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="H263">
         <v>0</v>
@@ -24501,7 +24504,7 @@
         <v>3617</v>
       </c>
       <c r="G264">
-        <v>10783200</v>
+        <v>0.16400000000000001</v>
       </c>
       <c r="H264">
         <v>870</v>
@@ -24577,7 +24580,7 @@
         <v>3926</v>
       </c>
       <c r="G265">
-        <v>5005410</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="H265">
         <v>0</v>
@@ -24653,7 +24656,7 @@
         <v>3458</v>
       </c>
       <c r="G266">
-        <v>20763600</v>
+        <v>0.372</v>
       </c>
       <c r="H266">
         <v>0</v>
@@ -24729,7 +24732,7 @@
         <v>3958</v>
       </c>
       <c r="G267">
-        <v>25685800</v>
+        <v>0.40400000000000003</v>
       </c>
       <c r="H267">
         <v>1195</v>
@@ -24805,7 +24808,7 @@
         <v>4245</v>
       </c>
       <c r="G268">
-        <v>29454300</v>
+        <v>0.45500000000000002</v>
       </c>
       <c r="H268">
         <v>1198</v>
@@ -24881,7 +24884,7 @@
         <v>3947</v>
       </c>
       <c r="G269">
-        <v>2021110</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="H269">
         <v>126</v>
@@ -24957,7 +24960,7 @@
         <v>4507</v>
       </c>
       <c r="G270">
-        <v>175481000</v>
+        <v>3.3010000000000002</v>
       </c>
       <c r="H270">
         <v>7876</v>
@@ -25033,7 +25036,7 @@
         <v>3804</v>
       </c>
       <c r="G271">
-        <v>310155000</v>
+        <v>2.3159999999999998</v>
       </c>
       <c r="H271">
         <v>11534</v>
@@ -25109,7 +25112,7 @@
         <v>1902</v>
       </c>
       <c r="G272">
-        <v>9119860</v>
+        <v>1.236</v>
       </c>
       <c r="H272">
         <v>0</v>
@@ -25185,7 +25188,7 @@
         <v>1987</v>
       </c>
       <c r="G273">
-        <v>16376300</v>
+        <v>1.754</v>
       </c>
       <c r="H273">
         <v>0</v>
@@ -25261,7 +25264,7 @@
         <v>2270</v>
       </c>
       <c r="G274">
-        <v>7624010</v>
+        <v>0.36299999999999999</v>
       </c>
       <c r="H274">
         <v>0</v>
@@ -25337,7 +25340,7 @@
         <v>2001</v>
       </c>
       <c r="G275">
-        <v>25676600</v>
+        <v>3.0209999999999999</v>
       </c>
       <c r="H275">
         <v>143</v>
@@ -25413,7 +25416,7 @@
         <v>2240</v>
       </c>
       <c r="G276">
-        <v>10852700</v>
+        <v>0.63200000000000001</v>
       </c>
       <c r="H276">
         <v>60</v>
@@ -25489,7 +25492,7 @@
         <v>2616</v>
       </c>
       <c r="G277">
-        <v>14411200</v>
+        <v>0.46899999999999997</v>
       </c>
       <c r="H277">
         <v>99</v>
@@ -25565,7 +25568,7 @@
         <v>2802</v>
       </c>
       <c r="G278">
-        <v>85759200</v>
+        <v>5.4859999999999998</v>
       </c>
       <c r="H278">
         <v>705</v>
@@ -25641,7 +25644,7 @@
         <v>1878</v>
       </c>
       <c r="G279">
-        <v>14171400</v>
+        <v>2.0019999999999998</v>
       </c>
       <c r="H279">
         <v>0</v>
@@ -25717,7 +25720,7 @@
         <v>1974</v>
       </c>
       <c r="G280">
-        <v>2044920</v>
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="H280">
         <v>0</v>
@@ -25793,7 +25796,7 @@
         <v>2038</v>
       </c>
       <c r="G281">
-        <v>5990950</v>
+        <v>0.23499999999999999</v>
       </c>
       <c r="H281">
         <v>0</v>
@@ -25869,7 +25872,7 @@
         <v>1883</v>
       </c>
       <c r="G282">
-        <v>12561600</v>
+        <v>1.5880000000000001</v>
       </c>
       <c r="H282">
         <v>0</v>
@@ -25945,7 +25948,7 @@
         <v>1976</v>
       </c>
       <c r="G283">
-        <v>36025800</v>
+        <v>5.23</v>
       </c>
       <c r="H283">
         <v>225</v>
@@ -26021,7 +26024,7 @@
         <v>2248</v>
       </c>
       <c r="G284">
-        <v>4769620</v>
+        <v>0.14299999999999999</v>
       </c>
       <c r="H284">
         <v>0</v>
@@ -26097,7 +26100,7 @@
         <v>2196</v>
       </c>
       <c r="G285">
-        <v>1587500</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="H285">
         <v>0</v>
@@ -26173,7 +26176,7 @@
         <v>2288</v>
       </c>
       <c r="G286">
-        <v>4033450</v>
+        <v>0.13900000000000001</v>
       </c>
       <c r="H286">
         <v>0</v>
@@ -26249,7 +26252,7 @@
         <v>2537</v>
       </c>
       <c r="G287">
-        <v>19538100</v>
+        <v>0.995</v>
       </c>
       <c r="H287">
         <v>104</v>
@@ -26325,7 +26328,7 @@
         <v>1875</v>
       </c>
       <c r="G288">
-        <v>15737200</v>
+        <v>2.431</v>
       </c>
       <c r="H288">
         <v>152</v>
@@ -26401,7 +26404,7 @@
         <v>2023</v>
       </c>
       <c r="G289">
-        <v>12068500</v>
+        <v>1.0589999999999999</v>
       </c>
       <c r="H289">
         <v>216</v>
@@ -26477,7 +26480,7 @@
         <v>2260</v>
       </c>
       <c r="G290">
-        <v>7773280</v>
+        <v>0.371</v>
       </c>
       <c r="H290">
         <v>26</v>
@@ -26553,7 +26556,7 @@
         <v>2434</v>
       </c>
       <c r="G291">
-        <v>20244300</v>
+        <v>0.755</v>
       </c>
       <c r="H291">
         <v>391</v>
@@ -26629,7 +26632,7 @@
         <v>3027</v>
       </c>
       <c r="G292">
-        <v>140249000</v>
+        <v>3.0609999999999999</v>
       </c>
       <c r="H292">
         <v>2085</v>
@@ -26705,7 +26708,7 @@
         <v>2673</v>
       </c>
       <c r="G293">
-        <v>11721000</v>
+        <v>0.22600000000000001</v>
       </c>
       <c r="H293">
         <v>211</v>
@@ -26781,7 +26784,7 @@
         <v>3378</v>
       </c>
       <c r="G294">
-        <v>66770000</v>
+        <v>1.282</v>
       </c>
       <c r="H294">
         <v>1052</v>
@@ -26857,7 +26860,7 @@
         <v>1892</v>
       </c>
       <c r="G295">
-        <v>21574300</v>
+        <v>2.1970000000000001</v>
       </c>
       <c r="H295">
         <v>0</v>
@@ -26933,7 +26936,7 @@
         <v>2124</v>
       </c>
       <c r="G296">
-        <v>10311700</v>
+        <v>0.46400000000000002</v>
       </c>
       <c r="H296">
         <v>0</v>
@@ -27009,7 +27012,7 @@
         <v>1805</v>
       </c>
       <c r="G297">
-        <v>21024600</v>
+        <v>3.984</v>
       </c>
       <c r="H297">
         <v>0</v>
@@ -27085,7 +27088,7 @@
         <v>2079</v>
       </c>
       <c r="G298">
-        <v>37171800</v>
+        <v>2.0419999999999998</v>
       </c>
       <c r="H298">
         <v>0</v>
@@ -27161,7 +27164,7 @@
         <v>2621</v>
       </c>
       <c r="G299">
-        <v>45892200</v>
+        <v>0.82899999999999996</v>
       </c>
       <c r="H299">
         <v>0</v>
@@ -27237,7 +27240,7 @@
         <v>1788</v>
       </c>
       <c r="G300">
-        <v>49161300</v>
+        <v>7.5609999999999999</v>
       </c>
       <c r="H300">
         <v>295</v>
@@ -27381,7 +27384,7 @@
         <v>1707</v>
       </c>
       <c r="G302">
-        <v>14147200</v>
+        <v>1.6220000000000001</v>
       </c>
       <c r="H302">
         <v>75</v>
@@ -27457,7 +27460,7 @@
         <v>1713</v>
       </c>
       <c r="G303">
-        <v>16730100</v>
+        <v>0.55400000000000005</v>
       </c>
       <c r="H303">
         <v>72</v>
@@ -27533,7 +27536,7 @@
         <v>1796</v>
       </c>
       <c r="G304">
-        <v>14640000</v>
+        <v>0.42</v>
       </c>
       <c r="H304">
         <v>194</v>
@@ -27609,7 +27612,7 @@
         <v>1830</v>
       </c>
       <c r="G305">
-        <v>36331300</v>
+        <v>1.02</v>
       </c>
       <c r="H305">
         <v>285</v>
@@ -27685,7 +27688,7 @@
         <v>1856</v>
       </c>
       <c r="G306">
-        <v>34385200</v>
+        <v>1.419</v>
       </c>
       <c r="H306">
         <v>259</v>
@@ -27761,7 +27764,7 @@
         <v>2030</v>
       </c>
       <c r="G307">
-        <v>25431100</v>
+        <v>1.105</v>
       </c>
       <c r="H307">
         <v>234</v>
@@ -27837,7 +27840,7 @@
         <v>1984</v>
       </c>
       <c r="G308">
-        <v>2854880</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="H308">
         <v>0</v>
@@ -27913,7 +27916,7 @@
         <v>2277</v>
       </c>
       <c r="G309">
-        <v>106853000</v>
+        <v>2.1179999999999999</v>
       </c>
       <c r="H309">
         <v>989</v>
@@ -27981,9 +27984,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R309"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L141" sqref="L141"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G46" sqref="G46:R55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27993,7 +27996,7 @@
     <col min="3" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.7109375" customWidth="1"/>
     <col min="6" max="6" width="6" customWidth="1"/>
-    <col min="7" max="7" width="5.140625" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" customWidth="1"/>
     <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
@@ -30279,19 +30282,19 @@
         <v>12</v>
       </c>
       <c r="H46" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="I46">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="J46">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="K46">
         <v>1</v>
       </c>
       <c r="L46">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="M46">
         <v>1</v>
@@ -30300,13 +30303,13 @@
         <v>1</v>
       </c>
       <c r="O46">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P46">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="Q46">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="R46">
         <v>1</v>
@@ -30329,19 +30332,19 @@
         <v>12</v>
       </c>
       <c r="H47" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="I47">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="J47">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="K47">
         <v>1</v>
       </c>
       <c r="L47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="M47">
         <v>1</v>
@@ -30350,13 +30353,13 @@
         <v>1</v>
       </c>
       <c r="O47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="Q47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="R47">
         <v>1</v>
@@ -30379,19 +30382,19 @@
         <v>12</v>
       </c>
       <c r="H48" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="I48">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="J48">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="K48">
         <v>1</v>
       </c>
       <c r="L48">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="M48">
         <v>1</v>
@@ -30400,13 +30403,13 @@
         <v>1</v>
       </c>
       <c r="O48">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P48">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="Q48">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="R48">
         <v>1</v>
@@ -30429,19 +30432,19 @@
         <v>12</v>
       </c>
       <c r="H49" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="I49">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="J49">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="K49">
         <v>1</v>
       </c>
       <c r="L49">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="M49">
         <v>1</v>
@@ -30450,13 +30453,13 @@
         <v>1</v>
       </c>
       <c r="O49">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P49">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="Q49">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="R49">
         <v>1</v>
@@ -30479,19 +30482,19 @@
         <v>13</v>
       </c>
       <c r="H50" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="I50">
         <v>0</v>
       </c>
       <c r="J50">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K50">
         <v>1</v>
       </c>
       <c r="L50">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="M50">
         <v>1</v>
@@ -30500,13 +30503,13 @@
         <v>1</v>
       </c>
       <c r="O50">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="P50">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="Q50">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="R50">
         <v>1</v>
@@ -30535,7 +30538,7 @@
         <v>0</v>
       </c>
       <c r="J51">
-        <v>1</v>
+        <v>15.5</v>
       </c>
       <c r="K51">
         <v>1</v>
@@ -30556,7 +30559,7 @@
         <v>1</v>
       </c>
       <c r="Q51">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R51">
         <v>1</v>
@@ -30585,7 +30588,7 @@
         <v>0</v>
       </c>
       <c r="J52">
-        <v>1</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="K52">
         <v>1</v>
@@ -30606,7 +30609,7 @@
         <v>1</v>
       </c>
       <c r="Q52">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R52">
         <v>1</v>
@@ -30629,19 +30632,19 @@
         <v>13</v>
       </c>
       <c r="H53" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="I53">
         <v>0</v>
       </c>
       <c r="J53">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K53">
         <v>1</v>
       </c>
       <c r="L53">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="M53">
         <v>1</v>
@@ -30650,13 +30653,13 @@
         <v>1</v>
       </c>
       <c r="O53">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="P53">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="Q53">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="R53">
         <v>1</v>
@@ -30679,19 +30682,19 @@
         <v>13</v>
       </c>
       <c r="H54" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="I54">
         <v>0</v>
       </c>
       <c r="J54">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K54">
         <v>1</v>
       </c>
       <c r="L54">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="M54">
         <v>1</v>
@@ -30700,13 +30703,13 @@
         <v>1</v>
       </c>
       <c r="O54">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="P54">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="Q54">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="R54">
         <v>1</v>
@@ -30729,19 +30732,19 @@
         <v>13</v>
       </c>
       <c r="H55" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="I55">
         <v>0</v>
       </c>
       <c r="J55">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K55">
         <v>1</v>
       </c>
       <c r="L55">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="M55">
         <v>1</v>
@@ -30750,13 +30753,13 @@
         <v>1</v>
       </c>
       <c r="O55">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="P55">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="Q55">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="R55">
         <v>1</v>
@@ -44999,8 +45002,8 @@
   <dimension ref="A1:R308"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A309" sqref="A309:XFD310"/>
+      <pane ySplit="1" topLeftCell="A170" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D169" sqref="D169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -53167,9 +53170,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:R152"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H95" sqref="H95"/>
+      <selection pane="bottomLeft" activeCell="J75" sqref="J75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -56240,11 +56243,11 @@
       </c>
       <c r="J3">
         <f>Catch2Wshed!$H$3*PRODUCT(Nodes!$K$50:$R$50)*PRODUCT(Nodes!$K$40:$R$40)</f>
-        <v>2094</v>
+        <v>65.4375</v>
       </c>
       <c r="K3">
         <f>Catch2Wshed!$I$3*PRODUCT(Nodes!$K$50:$S$50)*PRODUCT(Nodes!$K$40:$S$40)</f>
-        <v>864</v>
+        <v>27</v>
       </c>
       <c r="L3">
         <f>Catch2Wshed!$J$3*PRODUCT(Nodes!$K$50:$R$50)*PRODUCT(Nodes!$K$40:$R$40)</f>
@@ -56252,7 +56255,7 @@
       </c>
       <c r="M3">
         <f>Catch2Wshed!$K$3*PRODUCT(Nodes!$K$50:$R$50)*PRODUCT(Nodes!$K$40:$R$40)</f>
-        <v>2646</v>
+        <v>82.6875</v>
       </c>
       <c r="N3">
         <f>Catch2Wshed!$L$3*PRODUCT(Nodes!$K$50:$R$50)*PRODUCT(Nodes!$K$40:$R$40)</f>
@@ -56260,7 +56263,7 @@
       </c>
       <c r="O3">
         <f>Catch2Wshed!$M$3*PRODUCT(Nodes!$K$50:$R$50)*PRODUCT(Nodes!$K$40:$R$40)</f>
-        <v>792</v>
+        <v>24.75</v>
       </c>
       <c r="P3">
         <f>Catch2Wshed!$N$3*PRODUCT(Nodes!$K$50:$R$50)*PRODUCT(Nodes!$K$40:$R$40)</f>
@@ -56268,15 +56271,15 @@
       </c>
       <c r="Q3">
         <f>Catch2Wshed!$O$3*PRODUCT(Nodes!$K$50:$R$50)*PRODUCT(Nodes!$K$40:$R$40)</f>
-        <v>626</v>
+        <v>19.5625</v>
       </c>
       <c r="S3">
         <f>IFERROR(((J3-A3)/A3)*100, 0)</f>
-        <v>100</v>
+        <v>-93.75</v>
       </c>
       <c r="T3">
         <f t="shared" ref="T3:Z4" si="1">IFERROR(((K3-B3)/B3)*100, 0)</f>
-        <v>100</v>
+        <v>-93.75</v>
       </c>
       <c r="U3">
         <f t="shared" si="1"/>
@@ -56284,7 +56287,7 @@
       </c>
       <c r="V3">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>-93.75</v>
       </c>
       <c r="W3">
         <f t="shared" si="1"/>
@@ -56292,7 +56295,7 @@
       </c>
       <c r="X3">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>-93.75</v>
       </c>
       <c r="Y3">
         <f t="shared" si="1"/>
@@ -56300,7 +56303,7 @@
       </c>
       <c r="Z3">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>-93.75</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
@@ -56420,11 +56423,11 @@
       </c>
       <c r="J5">
         <f>Catch2Wshed!$H$5*PRODUCT(Nodes!$K$197:$R$197)*PRODUCT(Nodes!$K$50:$R$50)*PRODUCT(Nodes!$K$40:$R$40)</f>
-        <v>202.27199999999999</v>
+        <v>6.3209999999999997</v>
       </c>
       <c r="K5">
         <f>Catch2Wshed!$I$5*PRODUCT(Nodes!$K$197:$R$197)*PRODUCT(Nodes!$K$50:$R$50)*PRODUCT(Nodes!$K$40:$R$40)</f>
-        <v>4.5359999999999996</v>
+        <v>0.14174999999999999</v>
       </c>
       <c r="L5">
         <f>Catch2Wshed!$J$5*PRODUCT(Nodes!$K$197:$R$197)*PRODUCT(Nodes!$K$50:$R$50)*PRODUCT(Nodes!$K$40:$R$40)</f>
@@ -56432,7 +56435,7 @@
       </c>
       <c r="M5">
         <f>Catch2Wshed!$K$5*PRODUCT(Nodes!$K$197:$R$197)*PRODUCT(Nodes!$K$50:$R$50)*PRODUCT(Nodes!$K$40:$R$40)</f>
-        <v>90.719999999999985</v>
+        <v>2.8349999999999995</v>
       </c>
       <c r="N5">
         <f>Catch2Wshed!$L$5*PRODUCT(Nodes!$K$197:$R$197)*PRODUCT(Nodes!$K$50:$R$50)*PRODUCT(Nodes!$K$40:$R$40)</f>
@@ -56440,7 +56443,7 @@
       </c>
       <c r="O5">
         <f>Catch2Wshed!$M$5*PRODUCT(Nodes!$K$197:$R$197)*PRODUCT(Nodes!$K$50:$R$50)*PRODUCT(Nodes!$K$40:$R$40)</f>
-        <v>3.6959999999999997</v>
+        <v>0.11549999999999999</v>
       </c>
       <c r="P5">
         <f>Catch2Wshed!$N$5*PRODUCT(Nodes!$K$197:$R$197)*PRODUCT(Nodes!$K$50:$R$50)*PRODUCT(Nodes!$K$40:$R$40)</f>
@@ -56448,15 +56451,15 @@
       </c>
       <c r="Q5">
         <f>Catch2Wshed!$O$5*PRODUCT(Nodes!$K$197:$R$197)*PRODUCT(Nodes!$K$50:$R$50)*PRODUCT(Nodes!$K$40:$R$40)</f>
-        <v>3.3599999999999994</v>
+        <v>0.10499999999999998</v>
       </c>
       <c r="S5">
         <f>IFERROR(((J5-A5)/A5)*100, 0)</f>
-        <v>-83.2</v>
+        <v>-99.475000000000009</v>
       </c>
       <c r="T5">
         <f t="shared" ref="T5:T47" si="3">IFERROR(((K5-B5)/B5)*100, 0)</f>
-        <v>-83.2</v>
+        <v>-99.475000000000009</v>
       </c>
       <c r="U5">
         <f t="shared" ref="U5:U47" si="4">IFERROR(((L5-C5)/C5)*100, 0)</f>
@@ -56464,7 +56467,7 @@
       </c>
       <c r="V5">
         <f t="shared" ref="V5:V47" si="5">IFERROR(((M5-D5)/D5)*100, 0)</f>
-        <v>-83.2</v>
+        <v>-99.474999999999994</v>
       </c>
       <c r="W5">
         <f t="shared" ref="W5:W47" si="6">IFERROR(((N5-E5)/E5)*100, 0)</f>
@@ -56472,7 +56475,7 @@
       </c>
       <c r="X5">
         <f t="shared" ref="X5:X47" si="7">IFERROR(((O5-F5)/F5)*100, 0)</f>
-        <v>-83.2</v>
+        <v>-99.474999999999994</v>
       </c>
       <c r="Y5">
         <f t="shared" ref="Y5:Y47" si="8">IFERROR(((P5-G5)/G5)*100, 0)</f>
@@ -56480,7 +56483,7 @@
       </c>
       <c r="Z5">
         <f t="shared" ref="Z5:Z47" si="9">IFERROR(((Q5-H5)/H5)*100, 0)</f>
-        <v>-83.2</v>
+        <v>-99.475000000000009</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
@@ -56600,11 +56603,11 @@
       </c>
       <c r="J7">
         <f>Catch2Wshed!$H$7*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
-        <v>308</v>
+        <v>616</v>
       </c>
       <c r="K7">
         <f>Catch2Wshed!$I$7*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
-        <v>147</v>
+        <v>294</v>
       </c>
       <c r="L7">
         <f>Catch2Wshed!$J$7*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
@@ -56612,7 +56615,7 @@
       </c>
       <c r="M7">
         <f>Catch2Wshed!$K$7*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
-        <v>523</v>
+        <v>1046</v>
       </c>
       <c r="N7">
         <f>Catch2Wshed!$L$7*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
@@ -56620,7 +56623,7 @@
       </c>
       <c r="O7">
         <f>Catch2Wshed!$M$7*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
-        <v>126</v>
+        <v>252</v>
       </c>
       <c r="P7">
         <f>Catch2Wshed!$N$7*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
@@ -56628,15 +56631,15 @@
       </c>
       <c r="Q7">
         <f>Catch2Wshed!$O$7*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
-        <v>78</v>
+        <v>156</v>
       </c>
       <c r="S7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="T7">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="U7">
         <f t="shared" si="4"/>
@@ -56644,7 +56647,7 @@
       </c>
       <c r="V7">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="W7">
         <f t="shared" si="6"/>
@@ -56652,7 +56655,7 @@
       </c>
       <c r="X7">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="Y7">
         <f t="shared" si="8"/>
@@ -56660,7 +56663,7 @@
       </c>
       <c r="Z7">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
@@ -56690,11 +56693,11 @@
       </c>
       <c r="J8">
         <f>Catch2Wshed!$H$8*PRODUCT(Nodes!$K$230:$R$230)*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
-        <v>11.34</v>
+        <v>22.68</v>
       </c>
       <c r="K8">
         <f>Catch2Wshed!$I$8*PRODUCT(Nodes!$K$230:$R$230)*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
-        <v>2.0790000000000002</v>
+        <v>4.1580000000000004</v>
       </c>
       <c r="L8">
         <f>Catch2Wshed!$J$8*PRODUCT(Nodes!$K$230:$R$230)*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
@@ -56702,7 +56705,7 @@
       </c>
       <c r="M8">
         <f>Catch2Wshed!$K$8*PRODUCT(Nodes!$K$230:$R$230)*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
-        <v>9.0342000000000002</v>
+        <v>18.0684</v>
       </c>
       <c r="N8">
         <f>Catch2Wshed!$L$8*PRODUCT(Nodes!$K$230:$R$230)*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
@@ -56710,7 +56713,7 @@
       </c>
       <c r="O8">
         <f>Catch2Wshed!$M$8*PRODUCT(Nodes!$K$230:$R$230)*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
-        <v>1.7387999999999999</v>
+        <v>3.4775999999999998</v>
       </c>
       <c r="P8">
         <f>Catch2Wshed!$N$8*PRODUCT(Nodes!$K$230:$R$230)*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
@@ -56718,15 +56721,15 @@
       </c>
       <c r="Q8">
         <f>Catch2Wshed!$O$8*PRODUCT(Nodes!$K$230:$R$230)*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
-        <v>1.3608</v>
+        <v>2.7216</v>
       </c>
       <c r="S8">
         <f t="shared" si="2"/>
-        <v>-96.22</v>
+        <v>-92.44</v>
       </c>
       <c r="T8">
         <f t="shared" si="3"/>
-        <v>-96.22</v>
+        <v>-92.44</v>
       </c>
       <c r="U8">
         <f t="shared" si="4"/>
@@ -56734,7 +56737,7 @@
       </c>
       <c r="V8">
         <f t="shared" si="5"/>
-        <v>-96.22</v>
+        <v>-92.44</v>
       </c>
       <c r="W8">
         <f t="shared" si="6"/>
@@ -56742,7 +56745,7 @@
       </c>
       <c r="X8">
         <f t="shared" si="7"/>
-        <v>-96.22</v>
+        <v>-92.44</v>
       </c>
       <c r="Y8">
         <f t="shared" si="8"/>
@@ -56750,7 +56753,7 @@
       </c>
       <c r="Z8">
         <f t="shared" si="9"/>
-        <v>-96.22</v>
+        <v>-92.439999999999984</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
@@ -56870,11 +56873,11 @@
       </c>
       <c r="J10">
         <f>Catch2Wshed!$H$10*PRODUCT(Nodes!$K$193:$R$193)*PRODUCT(Nodes!$K$230:$R$230)*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
-        <v>7.5569759999999997</v>
+        <v>15.113951999999999</v>
       </c>
       <c r="K10">
         <f>Catch2Wshed!$I$10*PRODUCT(Nodes!$K$193:$R$193)*PRODUCT(Nodes!$K$230:$R$230)*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
-        <v>0.11748239999999999</v>
+        <v>0.23496479999999997</v>
       </c>
       <c r="L10">
         <f>Catch2Wshed!$J$10*PRODUCT(Nodes!$K$193:$R$193)*PRODUCT(Nodes!$K$230:$R$230)*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
@@ -56882,7 +56885,7 @@
       </c>
       <c r="M10">
         <f>Catch2Wshed!$K$10*PRODUCT(Nodes!$K$193:$R$193)*PRODUCT(Nodes!$K$230:$R$230)*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
-        <v>2.4671303999999994</v>
+        <v>4.9342607999999988</v>
       </c>
       <c r="N10">
         <f>Catch2Wshed!$L$10*PRODUCT(Nodes!$K$193:$R$193)*PRODUCT(Nodes!$K$230:$R$230)*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
@@ -56890,7 +56893,7 @@
       </c>
       <c r="O10">
         <f>Catch2Wshed!$M$10*PRODUCT(Nodes!$K$193:$R$193)*PRODUCT(Nodes!$K$230:$R$230)*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
-        <v>7.9379999999999992E-2</v>
+        <v>0.15875999999999998</v>
       </c>
       <c r="P10">
         <f>Catch2Wshed!$N$10*PRODUCT(Nodes!$K$193:$R$193)*PRODUCT(Nodes!$K$230:$R$230)*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
@@ -56898,15 +56901,15 @@
       </c>
       <c r="Q10">
         <f>Catch2Wshed!$O$10*PRODUCT(Nodes!$K$193:$R$193)*PRODUCT(Nodes!$K$230:$R$230)*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
-        <v>6.6679199999999994E-2</v>
+        <v>0.13335839999999999</v>
       </c>
       <c r="S10">
         <f t="shared" si="2"/>
-        <v>-99.682480000000012</v>
+        <v>-99.364959999999996</v>
       </c>
       <c r="T10">
         <f t="shared" si="3"/>
-        <v>-99.682479999999998</v>
+        <v>-99.364959999999996</v>
       </c>
       <c r="U10">
         <f t="shared" si="4"/>
@@ -56914,7 +56917,7 @@
       </c>
       <c r="V10">
         <f t="shared" si="5"/>
-        <v>-99.682480000000012</v>
+        <v>-99.364959999999996</v>
       </c>
       <c r="W10">
         <f t="shared" si="6"/>
@@ -56922,7 +56925,7 @@
       </c>
       <c r="X10">
         <f t="shared" si="7"/>
-        <v>-99.682479999999998</v>
+        <v>-99.364959999999996</v>
       </c>
       <c r="Y10">
         <f t="shared" si="8"/>
@@ -56930,7 +56933,7 @@
       </c>
       <c r="Z10">
         <f t="shared" si="9"/>
-        <v>-99.682480000000012</v>
+        <v>-99.364959999999996</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
@@ -56960,11 +56963,11 @@
       </c>
       <c r="J11">
         <f>Catch2Wshed!$H$11*PRODUCT(Nodes!$K$195:$R$195)*PRODUCT(Nodes!$K$230:$R$230)*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
-        <v>11.294186399999999</v>
+        <v>22.588372799999998</v>
       </c>
       <c r="K11">
         <f>Catch2Wshed!$I$11*PRODUCT(Nodes!$K$195:$R$195)*PRODUCT(Nodes!$K$230:$R$230)*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
-        <v>0.11430719999999998</v>
+        <v>0.22861439999999997</v>
       </c>
       <c r="L11">
         <f>Catch2Wshed!$J$11*PRODUCT(Nodes!$K$195:$R$195)*PRODUCT(Nodes!$K$230:$R$230)*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
@@ -56972,7 +56975,7 @@
       </c>
       <c r="M11">
         <f>Catch2Wshed!$K$11*PRODUCT(Nodes!$K$195:$R$195)*PRODUCT(Nodes!$K$230:$R$230)*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
-        <v>2.7306719999999998</v>
+        <v>5.4613439999999995</v>
       </c>
       <c r="N11">
         <f>Catch2Wshed!$L$11*PRODUCT(Nodes!$K$195:$R$195)*PRODUCT(Nodes!$K$230:$R$230)*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
@@ -56980,7 +56983,7 @@
       </c>
       <c r="O11">
         <f>Catch2Wshed!$M$11*PRODUCT(Nodes!$K$195:$R$195)*PRODUCT(Nodes!$K$230:$R$230)*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
-        <v>7.6204800000000003E-2</v>
+        <v>0.15240960000000001</v>
       </c>
       <c r="P11">
         <f>Catch2Wshed!$N$11*PRODUCT(Nodes!$K$195:$R$195)*PRODUCT(Nodes!$K$230:$R$230)*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
@@ -56988,15 +56991,15 @@
       </c>
       <c r="Q11">
         <f>Catch2Wshed!$O$11*PRODUCT(Nodes!$K$195:$R$195)*PRODUCT(Nodes!$K$230:$R$230)*PRODUCT(Nodes!$K$51:$R$51)*PRODUCT(Nodes!$K$43:$R$43)</f>
-        <v>6.3503999999999991E-2</v>
+        <v>0.12700799999999998</v>
       </c>
       <c r="S11">
         <f t="shared" si="2"/>
-        <v>-99.682480000000012</v>
+        <v>-99.364959999999996</v>
       </c>
       <c r="T11">
         <f t="shared" si="3"/>
-        <v>-99.682480000000012</v>
+        <v>-99.364959999999996</v>
       </c>
       <c r="U11">
         <f t="shared" si="4"/>
@@ -57004,7 +57007,7 @@
       </c>
       <c r="V11">
         <f t="shared" si="5"/>
-        <v>-99.682479999999998</v>
+        <v>-99.364959999999996</v>
       </c>
       <c r="W11">
         <f t="shared" si="6"/>
@@ -57012,7 +57015,7 @@
       </c>
       <c r="X11">
         <f t="shared" si="7"/>
-        <v>-99.682480000000012</v>
+        <v>-99.364959999999996</v>
       </c>
       <c r="Y11">
         <f t="shared" si="8"/>
@@ -57020,7 +57023,7 @@
       </c>
       <c r="Z11">
         <f t="shared" si="9"/>
-        <v>-99.682480000000012</v>
+        <v>-99.364959999999996</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
@@ -57140,11 +57143,11 @@
       </c>
       <c r="J13">
         <f>Catch2Wshed!$H$13*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
-        <v>99</v>
+        <v>198</v>
       </c>
       <c r="K13">
         <f>Catch2Wshed!$I$13*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="L13">
         <f>Catch2Wshed!$J$13*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
@@ -57152,7 +57155,7 @@
       </c>
       <c r="M13">
         <f>Catch2Wshed!$K$13*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
-        <v>142</v>
+        <v>284</v>
       </c>
       <c r="N13">
         <f>Catch2Wshed!$L$13*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
@@ -57160,7 +57163,7 @@
       </c>
       <c r="O13">
         <f>Catch2Wshed!$M$13*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="P13">
         <f>Catch2Wshed!$N$13*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
@@ -57168,15 +57171,15 @@
       </c>
       <c r="Q13">
         <f>Catch2Wshed!$O$13*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="S13">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="T13">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="U13">
         <f t="shared" si="4"/>
@@ -57184,7 +57187,7 @@
       </c>
       <c r="V13">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="W13">
         <f t="shared" si="6"/>
@@ -57192,7 +57195,7 @@
       </c>
       <c r="X13">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="Y13">
         <f t="shared" si="8"/>
@@ -57200,7 +57203,7 @@
       </c>
       <c r="Z13">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
@@ -57230,11 +57233,11 @@
       </c>
       <c r="J14">
         <f>Catch2Wshed!$H$14*PRODUCT(Nodes!$K$196:$R$196)*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
-        <v>15.203999999999999</v>
+        <v>30.407999999999998</v>
       </c>
       <c r="K14">
         <f>Catch2Wshed!$I$14*PRODUCT(Nodes!$K$196:$R$196)*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
-        <v>2.4359999999999999</v>
+        <v>4.8719999999999999</v>
       </c>
       <c r="L14">
         <f>Catch2Wshed!$J$14*PRODUCT(Nodes!$K$196:$R$196)*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
@@ -57242,7 +57245,7 @@
       </c>
       <c r="M14">
         <f>Catch2Wshed!$K$14*PRODUCT(Nodes!$K$196:$R$196)*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
-        <v>14.195999999999998</v>
+        <v>28.391999999999996</v>
       </c>
       <c r="N14">
         <f>Catch2Wshed!$L$14*PRODUCT(Nodes!$K$196:$R$196)*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
@@ -57250,7 +57253,7 @@
       </c>
       <c r="O14">
         <f>Catch2Wshed!$M$14*PRODUCT(Nodes!$K$196:$R$196)*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
-        <v>1.5959999999999999</v>
+        <v>3.1919999999999997</v>
       </c>
       <c r="P14">
         <f>Catch2Wshed!$N$14*PRODUCT(Nodes!$K$196:$R$196)*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
@@ -57258,15 +57261,15 @@
       </c>
       <c r="Q14">
         <f>Catch2Wshed!$O$14*PRODUCT(Nodes!$K$196:$R$196)*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
-        <v>1.0919999999999999</v>
+        <v>2.1839999999999997</v>
       </c>
       <c r="S14">
         <f t="shared" si="2"/>
-        <v>-91.6</v>
+        <v>-83.2</v>
       </c>
       <c r="T14">
         <f t="shared" si="3"/>
-        <v>-91.600000000000009</v>
+        <v>-83.2</v>
       </c>
       <c r="U14">
         <f t="shared" si="4"/>
@@ -57274,7 +57277,7 @@
       </c>
       <c r="V14">
         <f t="shared" si="5"/>
-        <v>-91.600000000000009</v>
+        <v>-83.2</v>
       </c>
       <c r="W14">
         <f t="shared" si="6"/>
@@ -57282,7 +57285,7 @@
       </c>
       <c r="X14">
         <f t="shared" si="7"/>
-        <v>-91.600000000000009</v>
+        <v>-83.2</v>
       </c>
       <c r="Y14">
         <f t="shared" si="8"/>
@@ -57290,7 +57293,7 @@
       </c>
       <c r="Z14">
         <f t="shared" si="9"/>
-        <v>-91.6</v>
+        <v>-83.2</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
@@ -57320,11 +57323,11 @@
       </c>
       <c r="J15">
         <f>Catch2Wshed!$H$15*PRODUCT(Nodes!$K$187:$R$187)*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
-        <v>0.41999999999999993</v>
+        <v>0.83999999999999986</v>
       </c>
       <c r="K15">
         <f>Catch2Wshed!$I$15*PRODUCT(Nodes!$K$187:$R$187)*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
-        <v>8.3999999999999991E-2</v>
+        <v>0.16799999999999998</v>
       </c>
       <c r="L15">
         <f>Catch2Wshed!$J$15*PRODUCT(Nodes!$K$187:$R$187)*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
@@ -57332,7 +57335,7 @@
       </c>
       <c r="M15">
         <f>Catch2Wshed!$K$15*PRODUCT(Nodes!$K$187:$R$187)*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
-        <v>0.33599999999999997</v>
+        <v>0.67199999999999993</v>
       </c>
       <c r="N15">
         <f>Catch2Wshed!$L$15*PRODUCT(Nodes!$K$187:$R$187)*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
@@ -57352,11 +57355,11 @@
       </c>
       <c r="S15">
         <f t="shared" si="2"/>
-        <v>-91.600000000000009</v>
+        <v>-83.2</v>
       </c>
       <c r="T15">
         <f t="shared" si="3"/>
-        <v>-91.600000000000009</v>
+        <v>-83.2</v>
       </c>
       <c r="U15">
         <f t="shared" si="4"/>
@@ -57364,7 +57367,7 @@
       </c>
       <c r="V15">
         <f t="shared" si="5"/>
-        <v>-91.600000000000009</v>
+        <v>-83.2</v>
       </c>
       <c r="W15">
         <f t="shared" si="6"/>
@@ -57500,11 +57503,11 @@
       </c>
       <c r="J17">
         <f>Catch2Wshed!$H$17*PRODUCT(Nodes!$K$189:$R$189)*PRODUCT(Nodes!$K$196:$R$196)*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
-        <v>11.338991999999999</v>
+        <v>22.677983999999999</v>
       </c>
       <c r="K17">
         <f>Catch2Wshed!$I$17*PRODUCT(Nodes!$K$189:$R$189)*PRODUCT(Nodes!$K$196:$R$196)*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
-        <v>0.23990399999999998</v>
+        <v>0.47980799999999996</v>
       </c>
       <c r="L17">
         <f>Catch2Wshed!$J$17*PRODUCT(Nodes!$K$189:$R$189)*PRODUCT(Nodes!$K$196:$R$196)*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
@@ -57512,7 +57515,7 @@
       </c>
       <c r="M17">
         <f>Catch2Wshed!$K$17*PRODUCT(Nodes!$K$189:$R$189)*PRODUCT(Nodes!$K$196:$R$196)*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
-        <v>6.1387199999999993</v>
+        <v>12.277439999999999</v>
       </c>
       <c r="N17">
         <f>Catch2Wshed!$L$17*PRODUCT(Nodes!$K$189:$R$189)*PRODUCT(Nodes!$K$196:$R$196)*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
@@ -57520,7 +57523,7 @@
       </c>
       <c r="O17">
         <f>Catch2Wshed!$M$17*PRODUCT(Nodes!$K$189:$R$189)*PRODUCT(Nodes!$K$196:$R$196)*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
-        <v>0.14111999999999997</v>
+        <v>0.28223999999999994</v>
       </c>
       <c r="P17">
         <f>Catch2Wshed!$N$17*PRODUCT(Nodes!$K$189:$R$189)*PRODUCT(Nodes!$K$196:$R$196)*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
@@ -57528,15 +57531,15 @@
       </c>
       <c r="Q17">
         <f>Catch2Wshed!H$17*PRODUCT(Nodes!$K$189:$R$189)*PRODUCT(Nodes!$K$196:$R$196)*PRODUCT(Nodes!$K$52:$R$52)*PRODUCT(Nodes!$K$45:$R$45)</f>
-        <v>11.338991999999999</v>
+        <v>22.677983999999999</v>
       </c>
       <c r="S17">
         <f t="shared" si="2"/>
-        <v>-99.29440000000001</v>
+        <v>-98.588800000000006</v>
       </c>
       <c r="T17">
         <f t="shared" si="3"/>
-        <v>-99.294399999999996</v>
+        <v>-98.588800000000006</v>
       </c>
       <c r="U17">
         <f t="shared" si="4"/>
@@ -57544,7 +57547,7 @@
       </c>
       <c r="V17">
         <f t="shared" si="5"/>
-        <v>-99.294399999999996</v>
+        <v>-98.588800000000006</v>
       </c>
       <c r="W17">
         <f t="shared" si="6"/>
@@ -57552,7 +57555,7 @@
       </c>
       <c r="X17">
         <f t="shared" si="7"/>
-        <v>-99.294399999999996</v>
+        <v>-98.588799999999992</v>
       </c>
       <c r="Y17">
         <f t="shared" si="8"/>
@@ -57560,7 +57563,7 @@
       </c>
       <c r="Z17">
         <f t="shared" si="9"/>
-        <v>-5.5084000000000053</v>
+        <v>88.983199999999982</v>
       </c>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.25">
@@ -60200,11 +60203,11 @@
       </c>
       <c r="J47">
         <f>Catch2Wshed!$H$47*PRODUCT(Nodes!$K$55:$R$55)*PRODUCT(Nodes!$K$35:$R$35)</f>
-        <v>1354</v>
+        <v>42.3125</v>
       </c>
       <c r="K47">
         <f>Catch2Wshed!$I$47*PRODUCT(Nodes!$K$55:$R$55)*PRODUCT(Nodes!$K$35:$R$35)</f>
-        <v>380</v>
+        <v>11.875</v>
       </c>
       <c r="L47">
         <f>Catch2Wshed!$J$47*PRODUCT(Nodes!$K$55:$R$55)*PRODUCT(Nodes!$K$35:$R$35)</f>
@@ -60212,7 +60215,7 @@
       </c>
       <c r="M47">
         <f>Catch2Wshed!$K$47*PRODUCT(Nodes!$K$55:$R$55)*PRODUCT(Nodes!$K$35:$R$35)</f>
-        <v>1714</v>
+        <v>53.5625</v>
       </c>
       <c r="N47">
         <f>Catch2Wshed!$L$47*PRODUCT(Nodes!$K$55:$R$55)*PRODUCT(Nodes!$K$35:$R$35)</f>
@@ -60220,7 +60223,7 @@
       </c>
       <c r="O47">
         <f>Catch2Wshed!$M$47*PRODUCT(Nodes!$K$55:$R$55)*PRODUCT(Nodes!$K$35:$R$35)</f>
-        <v>494</v>
+        <v>15.4375</v>
       </c>
       <c r="P47">
         <f>Catch2Wshed!$N$47*PRODUCT(Nodes!$K$55:$R$55)*PRODUCT(Nodes!$K$35:$R$35)</f>
@@ -60228,15 +60231,15 @@
       </c>
       <c r="Q47">
         <f>Catch2Wshed!$O$47*PRODUCT(Nodes!$K$55:$R$55)*PRODUCT(Nodes!$K$35:$R$35)</f>
-        <v>216</v>
+        <v>6.75</v>
       </c>
       <c r="S47">
         <f t="shared" si="2"/>
-        <v>100</v>
+        <v>-93.75</v>
       </c>
       <c r="T47">
         <f t="shared" si="3"/>
-        <v>100</v>
+        <v>-93.75</v>
       </c>
       <c r="U47">
         <f t="shared" si="4"/>
@@ -60244,7 +60247,7 @@
       </c>
       <c r="V47">
         <f t="shared" si="5"/>
-        <v>100</v>
+        <v>-93.75</v>
       </c>
       <c r="W47">
         <f t="shared" si="6"/>
@@ -60252,7 +60255,7 @@
       </c>
       <c r="X47">
         <f t="shared" si="7"/>
-        <v>100</v>
+        <v>-93.75</v>
       </c>
       <c r="Y47">
         <f t="shared" si="8"/>
@@ -60260,7 +60263,7 @@
       </c>
       <c r="Z47">
         <f t="shared" si="9"/>
-        <v>100</v>
+        <v>-93.75</v>
       </c>
     </row>
   </sheetData>
@@ -60307,11 +60310,11 @@
       </c>
       <c r="C2">
         <f>$B$2+($B$3*Nodes!$J$50)</f>
-        <v>189950600</v>
+        <v>75896200</v>
       </c>
       <c r="D2">
         <f>(($C$2-$B$2)/$B$2)*100</f>
-        <v>150.27682545371178</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -60369,11 +60372,11 @@
       </c>
       <c r="C6">
         <f>$B$6+($B$7*Nodes!$J$51)</f>
-        <v>70529500</v>
+        <v>609269750</v>
       </c>
       <c r="D6">
         <f>(($C$6-$B$6)/$B$6)*100</f>
-        <v>111.32434456928839</v>
+        <v>1725.5273408239698</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -60462,11 +60465,11 @@
       </c>
       <c r="C12">
         <f>$B$12+($B$13*Nodes!$J$52)</f>
-        <v>42016930</v>
+        <v>48789059</v>
       </c>
       <c r="D12">
         <f>(($C$12-$B$12)/$B$12)*100</f>
-        <v>14.15286516914985</v>
+        <v>32.551589889044649</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -60985,11 +60988,11 @@
       </c>
       <c r="C46">
         <f>$B$46+($B$47*Nodes!$J$55)</f>
-        <v>145225200</v>
+        <v>77894400</v>
       </c>
       <c r="D46">
         <f>(($C$46-$B$46)/$B$46)*100</f>
-        <v>86.438562977569632</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>